<commit_message>
Ensure all sector names are visible on the performance page
Update the API to correctly return all sector exposure data for display.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 54b95f43-839d-43a1-b23c-b8a21fe56cf6
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 60e00af6-480c-4cb1-a225-21913f10506a
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f473309e-b340-4b77-bcdf-327a8eec9336/54b95f43-839d-43a1-b23c-b8a21fe56cf6/UiOy98p
</commit_message>
<xml_diff>
--- a/LaserBeamExcel.xlsx
+++ b/LaserBeamExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://laserbeamptyltd.sharepoint.com/sites/LaserBeamCapital2/Shared Documents/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{5F60E2F0-575E-4A08-ABF9-32171979650C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12145B12-C231-4B03-B1D2-D9351D220D1E}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{5F60E2F0-575E-4A08-ABF9-32171979650C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53CE5253-0087-4283-9C94-44E87C04350C}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="684" windowWidth="24864" windowHeight="23628" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21168" yWindow="1380" windowWidth="24864" windowHeight="23628" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions - New month" sheetId="1" state="hidden" r:id="rId1"/>
@@ -981,11 +981,11 @@
     <numFmt numFmtId="175" formatCode="0.0;;;"/>
     <numFmt numFmtId="176" formatCode="0;;;"/>
     <numFmt numFmtId="177" formatCode="0%;\-0%;\ "/>
-    <numFmt numFmtId="180" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="&quot;$&quot;###&quot;b&quot;"/>
-    <numFmt numFmtId="182" formatCode="&quot;$&quot;###&quot;m&quot;"/>
-    <numFmt numFmtId="183" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="184" formatCode="[$-10409]#,##0.00;\(#,##0.00\);&quot;-&quot;"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="&quot;$&quot;###&quot;b&quot;"/>
+    <numFmt numFmtId="180" formatCode="&quot;$&quot;###&quot;m&quot;"/>
+    <numFmt numFmtId="181" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="182" formatCode="[$-10409]#,##0.00;\(#,##0.00\);&quot;-&quot;"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1391,7 +1391,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="21" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1712,21 +1712,6 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="22" fillId="5" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="169" fontId="34" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1745,25 +1730,25 @@
     <xf numFmtId="9" fontId="35" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="35" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="35" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="35" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="35" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="35" fillId="10" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="35" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="35" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="35" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="35" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="35" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="35" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="35" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1775,7 +1760,7 @@
     <xf numFmtId="43" fontId="36" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="184" fontId="36" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="36" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1784,7 +1769,7 @@
     <xf numFmtId="9" fontId="36" fillId="12" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="183" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -1796,19 +1781,13 @@
     <xf numFmtId="166" fontId="37" fillId="13" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="37" fillId="13" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="38" fillId="13" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="39" fillId="13" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="35" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="35" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="35" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
@@ -1823,13 +1802,35 @@
     <xf numFmtId="0" fontId="36" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="184" fontId="36" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="36" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="9" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="32" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="174" fontId="32" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="37" fillId="13" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="39" fillId="13" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="22" fillId="5" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7131,41 +7132,6 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="Monthly"/>
-      <sheetName val="Portfolio"/>
-      <sheetName val="Nov Perf"/>
-      <sheetName val="inception perf"/>
-      <sheetName val="Admin Fee"/>
-      <sheetName val="Quote Comparisons"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="41">
-          <cell r="G41">
-            <v>1.1200237411717677</v>
-          </cell>
-          <cell r="H41">
-            <v>1.1169995713674072</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
       <sheetName val="Instructions - New month"/>
       <sheetName val="Newsletter"/>
       <sheetName val="Performancedata"/>
@@ -7223,6 +7189,41 @@
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Monthly"/>
+      <sheetName val="Portfolio"/>
+      <sheetName val="Nov Perf"/>
+      <sheetName val="inception perf"/>
+      <sheetName val="Admin Fee"/>
+      <sheetName val="Quote Comparisons"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="41">
+          <cell r="G41">
+            <v>1.1200237411717677</v>
+          </cell>
+          <cell r="H41">
+            <v>1.1169995713674072</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7625,11 +7626,11 @@
     <row r="15" spans="1:1" ht="10.5" customHeight="1"/>
     <row r="16" spans="1:1" ht="6" customHeight="1"/>
     <row r="17" spans="2:15" ht="39.75" customHeight="1">
-      <c r="D17" s="132" t="s">
+      <c r="D17" s="166" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="132"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
       <c r="G17" s="10"/>
       <c r="H17" s="4" t="s">
         <v>10</v>
@@ -7650,11 +7651,11 @@
     </row>
     <row r="18" spans="2:15" ht="40.5" customHeight="1">
       <c r="B18" s="11"/>
-      <c r="D18" s="134" t="s">
+      <c r="D18" s="168" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="168"/>
       <c r="G18" s="12"/>
       <c r="H18" s="3">
         <f>INDEX(Performancedata!C:C, MATCH(A2, Performancedata!A:A, 0))</f>
@@ -7884,17 +7885,17 @@
     <row r="59" spans="2:24" ht="32.25" customHeight="1">
       <c r="B59" s="40"/>
       <c r="C59" s="17"/>
-      <c r="D59" s="132"/>
-      <c r="E59" s="132"/>
-      <c r="F59" s="132"/>
-      <c r="G59" s="132"/>
-      <c r="H59" s="132"/>
-      <c r="I59" s="132"/>
+      <c r="D59" s="166"/>
+      <c r="E59" s="166"/>
+      <c r="F59" s="166"/>
+      <c r="G59" s="166"/>
+      <c r="H59" s="166"/>
+      <c r="I59" s="166"/>
       <c r="J59" s="17"/>
-      <c r="K59" s="132"/>
-      <c r="L59" s="132"/>
-      <c r="M59" s="132"/>
-      <c r="N59" s="132"/>
+      <c r="K59" s="166"/>
+      <c r="L59" s="166"/>
+      <c r="M59" s="166"/>
+      <c r="N59" s="166"/>
       <c r="O59" s="10"/>
     </row>
     <row r="60" spans="2:24" ht="20.25" customHeight="1">
@@ -8071,41 +8072,41 @@
       <c r="AF111" s="10"/>
     </row>
     <row r="112" spans="19:32" ht="27.75" customHeight="1">
-      <c r="S112" s="133" t="s">
+      <c r="S112" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="T112" s="133"/>
+      <c r="T112" s="167"/>
       <c r="U112" s="30"/>
       <c r="V112" s="31"/>
       <c r="W112" s="31"/>
-      <c r="X112" s="133" t="s">
+      <c r="X112" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="Y112" s="133"/>
+      <c r="Y112" s="167"/>
       <c r="Z112" s="31"/>
       <c r="AA112" s="31"/>
       <c r="AB112" s="31"/>
-      <c r="AC112" s="133" t="s">
+      <c r="AC112" s="167" t="s">
         <v>19</v>
       </c>
-      <c r="AD112" s="133"/>
+      <c r="AD112" s="167"/>
       <c r="AE112" s="31"/>
       <c r="AF112" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="113" spans="19:33" ht="18.75" customHeight="1">
-      <c r="S113" s="133" t="s">
+      <c r="S113" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="T113" s="133"/>
+      <c r="T113" s="167"/>
       <c r="U113" s="30"/>
       <c r="V113" s="31"/>
       <c r="W113" s="31"/>
-      <c r="X113" s="133" t="s">
+      <c r="X113" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="Y113" s="133"/>
+      <c r="Y113" s="167"/>
       <c r="Z113" s="31"/>
       <c r="AA113" s="31"/>
       <c r="AB113" s="31"/>
@@ -8119,17 +8120,17 @@
       </c>
     </row>
     <row r="114" spans="19:33" ht="18.75" customHeight="1">
-      <c r="S114" s="133" t="s">
+      <c r="S114" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="T114" s="133"/>
+      <c r="T114" s="167"/>
       <c r="U114" s="30"/>
       <c r="V114" s="31"/>
       <c r="W114" s="31"/>
-      <c r="X114" s="133" t="s">
+      <c r="X114" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="Y114" s="133"/>
+      <c r="Y114" s="167"/>
       <c r="Z114" s="31"/>
       <c r="AA114" s="31"/>
       <c r="AB114" s="31"/>
@@ -8143,17 +8144,17 @@
       </c>
     </row>
     <row r="115" spans="19:33" ht="21.75" customHeight="1">
-      <c r="S115" s="133" t="s">
+      <c r="S115" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="T115" s="133"/>
+      <c r="T115" s="167"/>
       <c r="U115" s="45"/>
       <c r="V115" s="46"/>
       <c r="W115" s="46"/>
-      <c r="X115" s="133" t="s">
+      <c r="X115" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="Y115" s="133"/>
+      <c r="Y115" s="167"/>
       <c r="Z115" s="46"/>
       <c r="AA115" s="47"/>
       <c r="AB115" s="46"/>
@@ -8330,25 +8331,25 @@
       <c r="AE124" s="53"/>
     </row>
     <row r="125" spans="19:33" ht="26.5">
-      <c r="S125" s="132" t="s">
+      <c r="S125" s="166" t="s">
         <v>14</v>
       </c>
-      <c r="T125" s="132"/>
-      <c r="U125" s="132"/>
-      <c r="V125" s="132"/>
+      <c r="T125" s="166"/>
+      <c r="U125" s="166"/>
+      <c r="V125" s="166"/>
       <c r="W125" s="31"/>
-      <c r="X125" s="132" t="s">
+      <c r="X125" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="Y125" s="132"/>
-      <c r="Z125" s="132"/>
-      <c r="AA125" s="132"/>
-      <c r="AC125" s="132" t="s">
+      <c r="Y125" s="166"/>
+      <c r="Z125" s="166"/>
+      <c r="AA125" s="166"/>
+      <c r="AC125" s="166" t="s">
         <v>17</v>
       </c>
-      <c r="AD125" s="132"/>
-      <c r="AE125" s="132"/>
-      <c r="AF125" s="132"/>
+      <c r="AD125" s="166"/>
+      <c r="AE125" s="166"/>
+      <c r="AF125" s="166"/>
     </row>
     <row r="126" spans="19:33" ht="24">
       <c r="S126" s="2" t="s">
@@ -8477,12 +8478,12 @@
       </c>
     </row>
     <row r="131" spans="19:32" ht="26.5">
-      <c r="S131" s="132" t="s">
+      <c r="S131" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="T131" s="132"/>
-      <c r="U131" s="132"/>
-      <c r="V131" s="132"/>
+      <c r="T131" s="166"/>
+      <c r="U131" s="166"/>
+      <c r="V131" s="166"/>
       <c r="W131" s="31"/>
       <c r="X131" s="2" t="s">
         <v>48</v>
@@ -8722,80 +8723,80 @@
     <row r="1" spans="1:134" s="66" customFormat="1" ht="15.5">
       <c r="A1" s="63"/>
       <c r="B1" s="64"/>
-      <c r="C1" s="136" t="s">
+      <c r="C1" s="172" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
-      <c r="M1" s="136"/>
-      <c r="N1" s="136"/>
-      <c r="O1" s="136"/>
-      <c r="P1" s="136"/>
-      <c r="Q1" s="136"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="172"/>
+      <c r="J1" s="172"/>
+      <c r="K1" s="172"/>
+      <c r="L1" s="172"/>
+      <c r="M1" s="172"/>
+      <c r="N1" s="172"/>
+      <c r="O1" s="172"/>
+      <c r="P1" s="172"/>
+      <c r="Q1" s="172"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="136" t="s">
+      <c r="S1" s="172" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="136"/>
-      <c r="U1" s="136"/>
-      <c r="V1" s="136"/>
-      <c r="W1" s="136"/>
-      <c r="X1" s="136"/>
-      <c r="Y1" s="136"/>
-      <c r="Z1" s="136"/>
-      <c r="AA1" s="136"/>
-      <c r="AB1" s="136"/>
+      <c r="T1" s="172"/>
+      <c r="U1" s="172"/>
+      <c r="V1" s="172"/>
+      <c r="W1" s="172"/>
+      <c r="X1" s="172"/>
+      <c r="Y1" s="172"/>
+      <c r="Z1" s="172"/>
+      <c r="AA1" s="172"/>
+      <c r="AB1" s="172"/>
       <c r="AC1" s="1"/>
-      <c r="AD1" s="136" t="s">
+      <c r="AD1" s="172" t="s">
         <v>55</v>
       </c>
-      <c r="AE1" s="136"/>
-      <c r="AF1" s="136"/>
-      <c r="AG1" s="136"/>
-      <c r="AH1" s="136"/>
-      <c r="AI1" s="136"/>
-      <c r="AJ1" s="136"/>
-      <c r="AK1" s="136"/>
-      <c r="AL1" s="136"/>
-      <c r="AM1" s="136"/>
-      <c r="AN1" s="136"/>
+      <c r="AE1" s="172"/>
+      <c r="AF1" s="172"/>
+      <c r="AG1" s="172"/>
+      <c r="AH1" s="172"/>
+      <c r="AI1" s="172"/>
+      <c r="AJ1" s="172"/>
+      <c r="AK1" s="172"/>
+      <c r="AL1" s="172"/>
+      <c r="AM1" s="172"/>
+      <c r="AN1" s="172"/>
       <c r="AO1" s="1"/>
-      <c r="AP1" s="136" t="s">
+      <c r="AP1" s="172" t="s">
         <v>56</v>
       </c>
-      <c r="AQ1" s="136"/>
-      <c r="AR1" s="136"/>
-      <c r="AS1" s="136"/>
-      <c r="AT1" s="136"/>
-      <c r="AU1" s="136"/>
-      <c r="AV1" s="136"/>
-      <c r="AW1" s="136"/>
-      <c r="AX1" s="136"/>
+      <c r="AQ1" s="172"/>
+      <c r="AR1" s="172"/>
+      <c r="AS1" s="172"/>
+      <c r="AT1" s="172"/>
+      <c r="AU1" s="172"/>
+      <c r="AV1" s="172"/>
+      <c r="AW1" s="172"/>
+      <c r="AX1" s="172"/>
       <c r="AY1" s="1"/>
-      <c r="AZ1" s="136" t="s">
+      <c r="AZ1" s="172" t="s">
         <v>57</v>
       </c>
-      <c r="BA1" s="136"/>
-      <c r="BB1" s="136"/>
-      <c r="BC1" s="136"/>
-      <c r="BD1" s="136"/>
-      <c r="BE1" s="136"/>
-      <c r="BF1" s="136"/>
-      <c r="BG1" s="136"/>
-      <c r="BH1" s="136"/>
-      <c r="BI1" s="136"/>
-      <c r="BJ1" s="136"/>
-      <c r="BK1" s="136"/>
-      <c r="BL1" s="136"/>
-      <c r="BM1" s="136"/>
-      <c r="BN1" s="136"/>
+      <c r="BA1" s="172"/>
+      <c r="BB1" s="172"/>
+      <c r="BC1" s="172"/>
+      <c r="BD1" s="172"/>
+      <c r="BE1" s="172"/>
+      <c r="BF1" s="172"/>
+      <c r="BG1" s="172"/>
+      <c r="BH1" s="172"/>
+      <c r="BI1" s="172"/>
+      <c r="BJ1" s="172"/>
+      <c r="BK1" s="172"/>
+      <c r="BL1" s="172"/>
+      <c r="BM1" s="172"/>
+      <c r="BN1" s="172"/>
       <c r="BO1" s="1"/>
       <c r="BP1" s="65"/>
       <c r="BQ1" s="65"/>
@@ -8808,25 +8809,25 @@
       <c r="BX1" s="65"/>
       <c r="BY1" s="65"/>
       <c r="BZ1" s="65"/>
-      <c r="CA1" s="135"/>
-      <c r="CB1" s="135"/>
-      <c r="CC1" s="135"/>
-      <c r="CD1" s="135"/>
-      <c r="CE1" s="135"/>
-      <c r="CF1" s="135"/>
-      <c r="CG1" s="135"/>
-      <c r="CH1" s="135"/>
-      <c r="CI1" s="135"/>
-      <c r="CJ1" s="135"/>
-      <c r="CK1" s="135"/>
-      <c r="CL1" s="135"/>
-      <c r="CM1" s="135"/>
-      <c r="CN1" s="135"/>
-      <c r="CO1" s="135"/>
-      <c r="CP1" s="135"/>
-      <c r="CQ1" s="135"/>
-      <c r="CR1" s="135"/>
-      <c r="CS1" s="135"/>
+      <c r="CA1" s="171"/>
+      <c r="CB1" s="171"/>
+      <c r="CC1" s="171"/>
+      <c r="CD1" s="171"/>
+      <c r="CE1" s="171"/>
+      <c r="CF1" s="171"/>
+      <c r="CG1" s="171"/>
+      <c r="CH1" s="171"/>
+      <c r="CI1" s="171"/>
+      <c r="CJ1" s="171"/>
+      <c r="CK1" s="171"/>
+      <c r="CL1" s="171"/>
+      <c r="CM1" s="171"/>
+      <c r="CN1" s="171"/>
+      <c r="CO1" s="171"/>
+      <c r="CP1" s="171"/>
+      <c r="CQ1" s="171"/>
+      <c r="CR1" s="171"/>
+      <c r="CS1" s="171"/>
       <c r="DL1" s="67"/>
       <c r="DM1" s="65"/>
       <c r="DN1" s="65"/>
@@ -8836,247 +8837,247 @@
       <c r="DS1" s="67"/>
       <c r="DT1" s="67"/>
     </row>
-    <row r="2" spans="1:134" s="161" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A2" s="159" t="s">
+    <row r="2" spans="1:134" s="155" customFormat="1" ht="52.5" customHeight="1">
+      <c r="A2" s="154" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="159" t="s">
+      <c r="B2" s="154" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="159" t="s">
+      <c r="C2" s="154" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="159" t="s">
+      <c r="D2" s="154" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="159" t="s">
+      <c r="E2" s="154" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="159" t="s">
+      <c r="F2" s="154" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="159" t="s">
+      <c r="G2" s="154" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="159" t="s">
+      <c r="H2" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="159" t="s">
+      <c r="I2" s="154" t="s">
         <v>251</v>
       </c>
-      <c r="J2" s="159" t="s">
+      <c r="J2" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="159" t="s">
+      <c r="K2" s="154" t="s">
         <v>252</v>
       </c>
-      <c r="L2" s="159" t="s">
+      <c r="L2" s="154" t="s">
         <v>253</v>
       </c>
-      <c r="M2" s="159" t="s">
+      <c r="M2" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="159" t="s">
+      <c r="N2" s="154" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="159" t="s">
+      <c r="O2" s="154" t="s">
         <v>47</v>
       </c>
-      <c r="P2" s="159" t="s">
+      <c r="P2" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="159" t="s">
+      <c r="Q2" s="154" t="s">
         <v>254</v>
       </c>
-      <c r="R2" s="159" t="s">
+      <c r="R2" s="154" t="s">
         <v>255</v>
       </c>
-      <c r="S2" s="159" t="s">
+      <c r="S2" s="154" t="s">
         <v>67</v>
       </c>
-      <c r="T2" s="159" t="s">
+      <c r="T2" s="154" t="s">
         <v>68</v>
       </c>
-      <c r="U2" s="159" t="s">
+      <c r="U2" s="154" t="s">
         <v>69</v>
       </c>
-      <c r="V2" s="159" t="s">
+      <c r="V2" s="154" t="s">
         <v>70</v>
       </c>
-      <c r="W2" s="159" t="s">
+      <c r="W2" s="154" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="159" t="s">
+      <c r="X2" s="154" t="s">
         <v>66</v>
       </c>
-      <c r="Y2" s="159" t="s">
+      <c r="Y2" s="154" t="s">
         <v>256</v>
       </c>
-      <c r="Z2" s="159" t="s">
+      <c r="Z2" s="154" t="s">
         <v>257</v>
       </c>
-      <c r="AA2" s="159" t="s">
+      <c r="AA2" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="159" t="s">
+      <c r="AB2" s="154" t="s">
         <v>42</v>
       </c>
-      <c r="AC2" s="159"/>
-      <c r="AD2" s="159" t="s">
+      <c r="AC2" s="154"/>
+      <c r="AD2" s="154" t="s">
         <v>71</v>
       </c>
-      <c r="AE2" s="159" t="s">
+      <c r="AE2" s="154" t="s">
         <v>258</v>
       </c>
-      <c r="AF2" s="159" t="s">
+      <c r="AF2" s="154" t="s">
         <v>259</v>
       </c>
-      <c r="AG2" s="159" t="s">
+      <c r="AG2" s="154" t="s">
         <v>72</v>
       </c>
-      <c r="AH2" s="159" t="s">
+      <c r="AH2" s="154" t="s">
         <v>73</v>
       </c>
-      <c r="AI2" s="159" t="s">
+      <c r="AI2" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="AJ2" s="159" t="s">
+      <c r="AJ2" s="154" t="s">
         <v>75</v>
       </c>
-      <c r="AK2" s="159" t="s">
+      <c r="AK2" s="154" t="s">
         <v>260</v>
       </c>
-      <c r="AL2" s="159" t="s">
+      <c r="AL2" s="154" t="s">
         <v>261</v>
       </c>
-      <c r="AM2" s="159" t="s">
+      <c r="AM2" s="154" t="s">
         <v>262</v>
       </c>
-      <c r="AN2" s="159" t="s">
+      <c r="AN2" s="154" t="s">
         <v>263</v>
       </c>
-      <c r="AO2" s="159" t="s">
+      <c r="AO2" s="154" t="s">
         <v>78</v>
       </c>
-      <c r="AP2" s="159" t="s">
+      <c r="AP2" s="154" t="s">
         <v>264</v>
       </c>
-      <c r="AQ2" s="159" t="s">
+      <c r="AQ2" s="154" t="s">
         <v>265</v>
       </c>
-      <c r="AR2" s="159" t="s">
+      <c r="AR2" s="154" t="s">
         <v>266</v>
       </c>
-      <c r="AS2" s="159" t="s">
+      <c r="AS2" s="154" t="s">
         <v>267</v>
       </c>
-      <c r="AT2" s="159"/>
-      <c r="AU2" s="159"/>
-      <c r="AV2" s="159" t="s">
+      <c r="AT2" s="154"/>
+      <c r="AU2" s="154"/>
+      <c r="AV2" s="154" t="s">
         <v>72</v>
       </c>
-      <c r="AW2" s="159" t="s">
+      <c r="AW2" s="154" t="s">
         <v>73</v>
       </c>
-      <c r="AX2" s="159" t="s">
+      <c r="AX2" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="AY2" s="159" t="s">
+      <c r="AY2" s="154" t="s">
         <v>75</v>
       </c>
-      <c r="AZ2" s="159" t="s">
+      <c r="AZ2" s="154" t="s">
         <v>268</v>
       </c>
-      <c r="BA2" s="159" t="s">
+      <c r="BA2" s="154" t="s">
         <v>269</v>
       </c>
-      <c r="BB2" s="159" t="s">
+      <c r="BB2" s="154" t="s">
         <v>77</v>
       </c>
-      <c r="BC2" s="159" t="s">
+      <c r="BC2" s="154" t="s">
         <v>270</v>
       </c>
-      <c r="BD2" s="159" t="s">
+      <c r="BD2" s="154" t="s">
         <v>271</v>
       </c>
-      <c r="BE2" s="159"/>
-      <c r="BF2" s="159" t="s">
+      <c r="BE2" s="154"/>
+      <c r="BF2" s="154" t="s">
         <v>79</v>
       </c>
-      <c r="BG2" s="159" t="s">
+      <c r="BG2" s="154" t="s">
         <v>21</v>
       </c>
-      <c r="BH2" s="159" t="s">
+      <c r="BH2" s="154" t="s">
         <v>80</v>
       </c>
-      <c r="BI2" s="159" t="s">
+      <c r="BI2" s="154" t="s">
         <v>81</v>
       </c>
-      <c r="BJ2" s="159" t="s">
+      <c r="BJ2" s="154" t="s">
         <v>82</v>
       </c>
-      <c r="BK2" s="159" t="s">
+      <c r="BK2" s="154" t="s">
         <v>59</v>
       </c>
-      <c r="BL2" s="159" t="s">
+      <c r="BL2" s="154" t="s">
         <v>83</v>
       </c>
-      <c r="BM2" s="159" t="s">
+      <c r="BM2" s="154" t="s">
         <v>84</v>
       </c>
-      <c r="BN2" s="159" t="s">
+      <c r="BN2" s="154" t="s">
         <v>81</v>
       </c>
-      <c r="BO2" s="159" t="s">
+      <c r="BO2" s="154" t="s">
         <v>85</v>
       </c>
-      <c r="BP2" s="159" t="s">
+      <c r="BP2" s="154" t="s">
         <v>28</v>
       </c>
-      <c r="BQ2" s="159" t="s">
+      <c r="BQ2" s="154" t="s">
         <v>31</v>
       </c>
-      <c r="BR2" s="159" t="s">
+      <c r="BR2" s="154" t="s">
         <v>34</v>
       </c>
-      <c r="BS2" s="159" t="s">
+      <c r="BS2" s="154" t="s">
         <v>86</v>
       </c>
-      <c r="BT2" s="159" t="s">
+      <c r="BT2" s="154" t="s">
         <v>87</v>
       </c>
-      <c r="BU2" s="159" t="s">
+      <c r="BU2" s="154" t="s">
         <v>88</v>
       </c>
-      <c r="BV2" s="159" t="s">
+      <c r="BV2" s="154" t="s">
         <v>89</v>
       </c>
-      <c r="BW2" s="159"/>
-      <c r="BX2" s="160" t="s">
+      <c r="BW2" s="154"/>
+      <c r="BX2" s="169" t="s">
         <v>272</v>
       </c>
-      <c r="BY2" s="160"/>
-      <c r="BZ2" s="160"/>
-      <c r="CB2" s="162" t="s">
+      <c r="BY2" s="169"/>
+      <c r="BZ2" s="169"/>
+      <c r="CB2" s="170" t="s">
         <v>273</v>
       </c>
-      <c r="CC2" s="162"/>
+      <c r="CC2" s="170"/>
     </row>
     <row r="3" spans="1:134" s="56" customFormat="1" ht="15.5">
-      <c r="A3" s="137">
+      <c r="A3" s="132">
         <v>45838</v>
       </c>
-      <c r="B3" s="138">
+      <c r="B3" s="133">
         <v>1</v>
       </c>
-      <c r="C3" s="139"/>
-      <c r="D3" s="139">
+      <c r="C3" s="134"/>
+      <c r="D3" s="134">
         <v>0</v>
       </c>
-      <c r="E3" s="139"/>
-      <c r="F3" s="139"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="140"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="135"/>
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
@@ -9084,80 +9085,80 @@
       <c r="M3"/>
       <c r="N3"/>
       <c r="O3"/>
-      <c r="P3" s="158"/>
-      <c r="Q3" s="143"/>
-      <c r="R3" s="144">
-        <f>[2]Benchmarks!C3</f>
+      <c r="P3" s="153"/>
+      <c r="Q3" s="138"/>
+      <c r="R3" s="139">
+        <f>[1]Benchmarks!C3</f>
         <v>425.45</v>
       </c>
-      <c r="S3" s="139"/>
-      <c r="T3" s="139"/>
-      <c r="U3" s="140"/>
-      <c r="V3" s="158"/>
-      <c r="W3" s="139"/>
-      <c r="X3" s="141"/>
-      <c r="Y3" s="141"/>
-      <c r="Z3" s="141"/>
-      <c r="AA3" s="140"/>
-      <c r="AB3" s="140"/>
-      <c r="AC3" s="140"/>
-      <c r="AD3" s="139"/>
-      <c r="AE3" s="139"/>
-      <c r="AF3" s="139"/>
-      <c r="AG3" s="140"/>
-      <c r="AH3" s="140"/>
-      <c r="AI3" s="139"/>
-      <c r="AJ3" s="139"/>
-      <c r="AK3" s="139"/>
-      <c r="AL3" s="139"/>
-      <c r="AM3" s="139"/>
-      <c r="AN3" s="139"/>
-      <c r="AO3" s="139"/>
-      <c r="AP3" s="139"/>
-      <c r="AQ3" s="139"/>
-      <c r="AR3" s="139"/>
-      <c r="AS3" s="139"/>
-      <c r="AT3" s="139"/>
-      <c r="AU3" s="140"/>
-      <c r="AV3" s="140"/>
-      <c r="AW3" s="140"/>
-      <c r="AX3" s="139"/>
-      <c r="AY3" s="139"/>
-      <c r="AZ3" s="139"/>
-      <c r="BA3" s="139"/>
-      <c r="BB3" s="139"/>
-      <c r="BC3" s="139"/>
-      <c r="BD3" s="139"/>
-      <c r="BE3" s="140"/>
-      <c r="BF3" s="145"/>
-      <c r="BG3" s="146"/>
-      <c r="BH3" s="147"/>
-      <c r="BI3" s="140"/>
-      <c r="BJ3" s="140"/>
-      <c r="BK3" s="146"/>
-      <c r="BL3" s="146"/>
-      <c r="BM3" s="146"/>
-      <c r="BN3" s="146"/>
-      <c r="BO3" s="163"/>
-      <c r="BP3" s="164"/>
-      <c r="BQ3" s="164"/>
-      <c r="BR3" s="164"/>
-      <c r="BS3" s="163"/>
-      <c r="BT3" s="163"/>
-      <c r="BU3" s="150"/>
-      <c r="BV3" s="150"/>
-      <c r="BW3" s="150"/>
-      <c r="BX3" s="165" t="s">
+      <c r="S3" s="134"/>
+      <c r="T3" s="134"/>
+      <c r="U3" s="135"/>
+      <c r="V3" s="153"/>
+      <c r="W3" s="134"/>
+      <c r="X3" s="136"/>
+      <c r="Y3" s="136"/>
+      <c r="Z3" s="136"/>
+      <c r="AA3" s="135"/>
+      <c r="AB3" s="135"/>
+      <c r="AC3" s="135"/>
+      <c r="AD3" s="134"/>
+      <c r="AE3" s="134"/>
+      <c r="AF3" s="134"/>
+      <c r="AG3" s="135"/>
+      <c r="AH3" s="135"/>
+      <c r="AI3" s="134"/>
+      <c r="AJ3" s="134"/>
+      <c r="AK3" s="134"/>
+      <c r="AL3" s="134"/>
+      <c r="AM3" s="134"/>
+      <c r="AN3" s="134"/>
+      <c r="AO3" s="134"/>
+      <c r="AP3" s="134"/>
+      <c r="AQ3" s="134"/>
+      <c r="AR3" s="134"/>
+      <c r="AS3" s="134"/>
+      <c r="AT3" s="134"/>
+      <c r="AU3" s="135"/>
+      <c r="AV3" s="135"/>
+      <c r="AW3" s="135"/>
+      <c r="AX3" s="134"/>
+      <c r="AY3" s="134"/>
+      <c r="AZ3" s="134"/>
+      <c r="BA3" s="134"/>
+      <c r="BB3" s="134"/>
+      <c r="BC3" s="134"/>
+      <c r="BD3" s="134"/>
+      <c r="BE3" s="135"/>
+      <c r="BF3" s="140"/>
+      <c r="BG3" s="141"/>
+      <c r="BH3" s="142"/>
+      <c r="BI3" s="135"/>
+      <c r="BJ3" s="135"/>
+      <c r="BK3" s="141"/>
+      <c r="BL3" s="141"/>
+      <c r="BM3" s="141"/>
+      <c r="BN3" s="141"/>
+      <c r="BO3" s="156"/>
+      <c r="BP3" s="157"/>
+      <c r="BQ3" s="157"/>
+      <c r="BR3" s="157"/>
+      <c r="BS3" s="156"/>
+      <c r="BT3" s="156"/>
+      <c r="BU3" s="145"/>
+      <c r="BV3" s="145"/>
+      <c r="BW3" s="145"/>
+      <c r="BX3" s="158" t="s">
         <v>81</v>
       </c>
-      <c r="BY3" s="152" t="e">
+      <c r="BY3" s="147" t="e">
         <f>BZ3/$BZ$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BZ3" s="166">
+      <c r="BZ3" s="159">
         <v>17068298.050000001</v>
       </c>
-      <c r="CB3" s="167" t="s">
+      <c r="CB3" s="160" t="s">
         <v>170</v>
       </c>
       <c r="CD3" s="56" t="s">
@@ -9169,299 +9170,299 @@
       <c r="CF3" s="56" t="s">
         <v>275</v>
       </c>
-      <c r="CG3" s="155">
+      <c r="CG3" s="150">
         <v>6.0051455235897749E-2</v>
       </c>
-      <c r="CI3" s="156" cm="1">
+      <c r="CI3" s="151" cm="1">
         <f t="array" ref="CI3">_xll.BDP(CF3,"CUR_MKT_CAP","CURRENCY","AUD")</f>
         <v>3863262380000</v>
       </c>
-      <c r="CJ3" s="156">
+      <c r="CJ3" s="151">
         <v>3439516769999.9995</v>
       </c>
-      <c r="CK3" s="157" t="e">
+      <c r="CK3" s="152" t="e">
         <f>CG3/$CG$16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:134" s="56" customFormat="1" ht="15.5">
-      <c r="A4" s="137">
+      <c r="A4" s="132">
         <v>45869</v>
       </c>
-      <c r="B4" s="138">
+      <c r="B4" s="133">
         <v>1.0266</v>
       </c>
-      <c r="C4" s="139">
+      <c r="C4" s="134">
         <f>B4/B3-1</f>
         <v>2.6599999999999957E-2</v>
       </c>
-      <c r="D4" s="139">
+      <c r="D4" s="134">
         <f>((1+C4)*(1))-1</f>
         <v>2.6599999999999957E-2</v>
       </c>
-      <c r="E4" s="139"/>
-      <c r="F4" s="139">
+      <c r="E4" s="134"/>
+      <c r="F4" s="134">
         <f>D4</f>
         <v>2.6599999999999957E-2</v>
       </c>
-      <c r="G4" s="139">
+      <c r="G4" s="134">
         <f>D4</f>
         <v>2.6599999999999957E-2</v>
       </c>
-      <c r="H4" s="140">
+      <c r="H4" s="135">
         <f>((1+D4)^(365/(_xlfn.DAYS(A4,"1/07/2025"))))-1</f>
         <v>0.37630703279551914</v>
       </c>
-      <c r="I4" s="139" t="str">
+      <c r="I4" s="134" t="str">
         <f>IFERROR(_xlfn.STDEV.S($C$4:C4)*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="J4" s="141" t="str">
+      <c r="J4" s="136" t="str">
         <f>IFERROR(SUMIF(C$4:C4,"&gt;0",C$4:C4)/ABS(SUMIF(C$4:C4,"&lt;0",C$4:C4)),"")</f>
         <v/>
       </c>
-      <c r="K4" s="158" t="str">
+      <c r="K4" s="153" t="str">
         <f>IFERROR(AVERAGE($AG$4:AG4)/AK4*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="L4" s="141" t="str">
+      <c r="L4" s="136" t="str">
         <f>IFERROR(AVERAGE($AG$4:AG4)/_xlfn.STDEV.S($AG$4:AG4)*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="M4" s="139">
+      <c r="M4" s="134">
         <f>MAX($C$4:C4)</f>
         <v>2.6599999999999957E-2</v>
       </c>
-      <c r="N4" s="139">
+      <c r="N4" s="134">
         <f>MIN($C$4:C4)</f>
         <v>2.6599999999999957E-2</v>
       </c>
-      <c r="O4" s="140">
+      <c r="O4" s="135">
         <f>IFERROR(AVERAGEIF($S$4:S4,"&gt;0",$C$4:C4)/AVERAGEIF($S$4:S4,"&gt;0",$S$4:S4),"")</f>
         <v>0.83891549295774359</v>
       </c>
-      <c r="P4" s="158" t="str">
+      <c r="P4" s="153" t="str">
         <f>IFERROR(AVERAGEIF($S$4:S4,"&lt;0",$C$4:C4)/AVERAGEIF($S$4:S4,"&lt;0",$S$4:S4),"-")</f>
         <v>-</v>
       </c>
-      <c r="Q4" s="143" t="str">
+      <c r="Q4" s="138" t="str">
         <f>IFERROR(SLOPE($C$4:C4,$S$4:S4),"")</f>
         <v/>
       </c>
-      <c r="R4" s="144">
-        <f>[2]Benchmarks!C4</f>
+      <c r="R4" s="139">
+        <f>[1]Benchmarks!C4</f>
         <v>438.94</v>
       </c>
-      <c r="S4" s="139">
+      <c r="S4" s="134">
         <f>R4/R3-1</f>
         <v>3.1707603713714949E-2</v>
       </c>
-      <c r="T4" s="139">
+      <c r="T4" s="134">
         <f>((1+S4)*(1+T3))-1</f>
         <v>3.1707603713714949E-2</v>
       </c>
-      <c r="U4" s="140"/>
-      <c r="V4" s="142">
+      <c r="U4" s="135"/>
+      <c r="V4" s="137">
         <f t="shared" ref="V4:V8" si="0">((1+T4)^(365/(_xlfn.DAYS(A4,"30/06/2025"))))-1</f>
         <v>0.44417027234833251</v>
       </c>
-      <c r="W4" s="139" t="str">
+      <c r="W4" s="134" t="str">
         <f>IFERROR(STDEV($S$4:S4),"")</f>
         <v/>
       </c>
-      <c r="X4" s="141" t="str">
+      <c r="X4" s="136" t="str">
         <f>IFERROR(SUMIF(S$4:S4,"&gt;0",S$4:S4)/ABS(SUMIF(S$4:S4,"&lt;0",S$4:S4)),"")</f>
         <v/>
       </c>
-      <c r="Y4" s="158" t="str">
+      <c r="Y4" s="153" t="str">
         <f>IFERROR(AVERAGE($AV$4:AV4)/AZ4*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="Z4" s="141" t="str">
+      <c r="Z4" s="136" t="str">
         <f>IFERROR(AVERAGE($AV$4:AV4)/_xlfn.STDEV.S($AV$4:AV4)*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="AA4" s="139">
+      <c r="AA4" s="134">
         <f>MAX($S$4:S4)</f>
         <v>3.1707603713714949E-2</v>
       </c>
-      <c r="AB4" s="139">
+      <c r="AB4" s="134">
         <f>MIN($S$4:S4)</f>
         <v>3.1707603713714949E-2</v>
       </c>
-      <c r="AC4" s="140"/>
-      <c r="AD4" s="139">
+      <c r="AC4" s="135"/>
+      <c r="AD4" s="134">
         <v>0</v>
       </c>
-      <c r="AE4" s="139">
+      <c r="AE4" s="134">
         <v>3.85E-2</v>
       </c>
-      <c r="AF4" s="139">
+      <c r="AF4" s="134">
         <f>((1+AE4)^(1/12))-1</f>
         <v>3.1530742084739938E-3</v>
       </c>
-      <c r="AG4" s="140">
+      <c r="AG4" s="135">
         <f>C4-AF4</f>
         <v>2.3446925791525963E-2</v>
       </c>
-      <c r="AH4" s="140">
+      <c r="AH4" s="135">
         <f>G4-(AF4*12)</f>
         <v>-1.1236890501687968E-2</v>
       </c>
-      <c r="AI4" s="139" t="str">
+      <c r="AI4" s="134" t="str">
         <f>IF(AG4&lt;0, AG4, "")</f>
         <v/>
       </c>
-      <c r="AJ4" s="139">
+      <c r="AJ4" s="134">
         <f>IFERROR(AI4*AI4,0)</f>
         <v>0</v>
       </c>
-      <c r="AK4" s="139" cm="1">
+      <c r="AK4" s="134" cm="1">
         <f t="array" ref="AK4">IFERROR(SQRT(AVERAGE(IF($AG$4:AG4&lt;0,($AG$4:AG4)^2,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="AL4" s="139">
+      <c r="AL4" s="134">
         <f>IFERROR(AK4*SQRT(12),"")</f>
         <v>0</v>
       </c>
-      <c r="AM4" s="139">
+      <c r="AM4" s="134">
         <f>IFERROR(AVERAGE($AG$4:AG4),"")</f>
         <v>2.3446925791525963E-2</v>
       </c>
-      <c r="AN4" s="139" t="str">
+      <c r="AN4" s="134" t="str">
         <f>IFERROR(_xlfn.STDEV.S($AG$4:AG4),"")</f>
         <v/>
       </c>
-      <c r="AO4" s="139" t="str">
+      <c r="AO4" s="134" t="str">
         <f>IFERROR(AM4/AN4*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="AP4" s="139" t="str">
+      <c r="AP4" s="134" t="str">
         <f>IFERROR(CORREL($C$4:C4,$S$4:S4),"")</f>
         <v/>
       </c>
-      <c r="AQ4" s="139" t="str">
+      <c r="AQ4" s="134" t="str">
         <f>IFERROR(RSQ($C$4:C4,$S$4:S4),"")</f>
         <v/>
       </c>
-      <c r="AR4" s="139" t="str" cm="1">
+      <c r="AR4" s="134" t="str" cm="1">
         <f t="array" ref="AR4">IFERROR(_xlfn.STDEV.S($C$4:C4-$S$4:S4)*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="AS4" s="139" t="str" cm="1">
+      <c r="AS4" s="134" t="str" cm="1">
         <f t="array" ref="AS4">IFERROR((AVERAGE($C$4:C4-$S$4:S4)*12)/(_xlfn.STDEV.S($C$4:C4-$S$4:S4)*SQRT(12)),"")</f>
         <v/>
       </c>
-      <c r="AT4" s="139"/>
-      <c r="AU4" s="140"/>
-      <c r="AV4" s="140">
+      <c r="AT4" s="134"/>
+      <c r="AU4" s="135"/>
+      <c r="AV4" s="135">
         <f>S4-AF4</f>
         <v>2.8554529505240955E-2</v>
       </c>
-      <c r="AW4" s="140">
+      <c r="AW4" s="135">
         <f>U4-(AF4*12)</f>
         <v>-3.7836890501687925E-2</v>
       </c>
-      <c r="AX4" s="139" t="str">
+      <c r="AX4" s="134" t="str">
         <f t="shared" ref="AX4:AX8" si="1">IF(AV4&lt;0, AV4, "")</f>
         <v/>
       </c>
-      <c r="AY4" s="139">
+      <c r="AY4" s="134">
         <f t="shared" ref="AY4:AY8" si="2">IFERROR(AX4*AX4,0)</f>
         <v>0</v>
       </c>
-      <c r="AZ4" s="139" cm="1">
+      <c r="AZ4" s="134" cm="1">
         <f t="array" ref="AZ4">IFERROR(SQRT(AVERAGE(IF($AV$4:AV4&lt;0,($AV$4:AV4)^2,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="BA4" s="139">
+      <c r="BA4" s="134">
         <f>IFERROR(AZ4*SQRT(12),"")</f>
         <v>0</v>
       </c>
-      <c r="BB4" s="139">
+      <c r="BB4" s="134">
         <f t="shared" ref="BB4:BB8" si="3">IFERROR(AV4*AV4,0)</f>
         <v>8.1536115526567631E-4</v>
       </c>
-      <c r="BC4" s="139" t="str">
+      <c r="BC4" s="134" t="str">
         <f>IFERROR(_xlfn.STDEV.S($AV$4:AV4),"")</f>
         <v/>
       </c>
-      <c r="BD4" s="139" t="str">
+      <c r="BD4" s="134" t="str">
         <f>IFERROR(BC4*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="BE4" s="140"/>
-      <c r="BF4" s="145"/>
-      <c r="BG4" s="146"/>
-      <c r="BH4" s="147"/>
-      <c r="BI4" s="140">
+      <c r="BE4" s="135"/>
+      <c r="BF4" s="140"/>
+      <c r="BG4" s="141"/>
+      <c r="BH4" s="142"/>
+      <c r="BI4" s="135">
         <f>BN4/BK4</f>
         <v>0.76509667506176826</v>
       </c>
-      <c r="BJ4" s="140">
+      <c r="BJ4" s="135">
         <f>AVERAGE($BI$4:BI4)</f>
         <v>0.76509667506176826</v>
       </c>
-      <c r="BK4" s="148">
+      <c r="BK4" s="143">
         <v>14435005</v>
       </c>
-      <c r="BL4" s="148">
+      <c r="BL4" s="143">
         <v>3335141</v>
       </c>
-      <c r="BM4" s="148">
+      <c r="BM4" s="143">
         <v>55688</v>
       </c>
-      <c r="BN4" s="148">
+      <c r="BN4" s="143">
         <v>11044174.33</v>
       </c>
-      <c r="BO4" s="149">
+      <c r="BO4" s="144">
         <f>BL4+BM4</f>
         <v>3390829</v>
       </c>
-      <c r="BP4" s="149">
+      <c r="BP4" s="144">
         <f>BL4-BM4</f>
         <v>3279453</v>
       </c>
-      <c r="BQ4" s="142">
+      <c r="BQ4" s="137">
         <f>BL4/BK4</f>
         <v>0.23104536506914961</v>
       </c>
-      <c r="BR4" s="142">
+      <c r="BR4" s="137">
         <f>-BM4/BK4</f>
         <v>-3.857844178093461E-3</v>
       </c>
-      <c r="BS4" s="142">
+      <c r="BS4" s="137">
         <f>BO4/BK4</f>
         <v>0.23490320924724306</v>
       </c>
-      <c r="BT4" s="142">
+      <c r="BT4" s="137">
         <f>BP4/BK4</f>
         <v>0.22718752089105615</v>
       </c>
-      <c r="BU4" s="142">
+      <c r="BU4" s="137">
         <f>AVERAGE($BS$4:BS4)</f>
         <v>0.23490320924724306</v>
       </c>
-      <c r="BV4" s="142">
+      <c r="BV4" s="137">
         <f>AVERAGE($BT$4:BT4)</f>
         <v>0.22718752089105615</v>
       </c>
-      <c r="BW4" s="150"/>
-      <c r="BX4" s="168" t="s">
+      <c r="BW4" s="145"/>
+      <c r="BX4" s="161" t="s">
         <v>106</v>
       </c>
-      <c r="BY4" s="152" t="e">
+      <c r="BY4" s="147" t="e">
         <f>BZ4/$BZ$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BZ4" s="169">
+      <c r="BZ4" s="162">
         <v>1412895.3399499999</v>
       </c>
       <c r="CB4" s="84" t="e">
         <f>"&gt;$10b (" &amp; TEXT(CC4,"0%") &amp; ")"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="CC4" s="170" t="e" cm="1">
+      <c r="CC4" s="163" t="e" cm="1">
         <f t="array" ref="CC4">SUMPRODUCT((CJ$3:CJ$15&gt;=10000000000)*CK$3:CK$15)</f>
         <v>#DIV/0!</v>
       </c>
@@ -9474,302 +9475,302 @@
       <c r="CF4" s="56" t="s">
         <v>278</v>
       </c>
-      <c r="CG4" s="155">
+      <c r="CG4" s="150">
         <v>5.4955812545733819E-2</v>
       </c>
-      <c r="CI4" s="156" cm="1">
+      <c r="CI4" s="151" cm="1">
         <f t="array" ref="CI4">_xll.BDP(CF4,"CUR_MKT_CAP","CURRENCY","AUD")</f>
         <v>110529938395.65999</v>
       </c>
-      <c r="CJ4" s="156">
+      <c r="CJ4" s="151">
         <v>118757636055.37999</v>
       </c>
-      <c r="CK4" s="157" t="e">
+      <c r="CK4" s="152" t="e">
         <f>CG4/$CG$16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:134" s="56" customFormat="1" ht="15.5">
-      <c r="A5" s="137">
+      <c r="A5" s="132">
         <v>45900</v>
       </c>
-      <c r="B5" s="138">
+      <c r="B5" s="133">
         <v>1.0504</v>
       </c>
-      <c r="C5" s="139">
+      <c r="C5" s="134">
         <f>B5/B4-1</f>
         <v>2.3183323592441019E-2</v>
       </c>
-      <c r="D5" s="139">
+      <c r="D5" s="134">
         <f>((1+C5)*(1+D4))-1</f>
         <v>5.04E-2</v>
       </c>
-      <c r="E5" s="139">
+      <c r="E5" s="134">
         <f>((1+C5)*(1+C4)*(1+C3)-1)</f>
         <v>5.04E-2</v>
       </c>
-      <c r="F5" s="139">
+      <c r="F5" s="134">
         <f t="shared" ref="F5" si="4">D5</f>
         <v>5.04E-2</v>
       </c>
-      <c r="G5" s="139">
+      <c r="G5" s="134">
         <f t="shared" ref="G5" si="5">D5</f>
         <v>5.04E-2</v>
       </c>
-      <c r="H5" s="140">
+      <c r="H5" s="135">
         <f>((1+D5)^(365/(_xlfn.DAYS(A5,"1/07/2025"))))-1</f>
         <v>0.34207937198549043</v>
       </c>
-      <c r="I5" s="139">
+      <c r="I5" s="134">
         <f>IFERROR(_xlfn.STDEV.S($C$4:C5)*SQRT(12),"")</f>
         <v>8.3691138147248961E-3</v>
       </c>
-      <c r="J5" s="141" t="str">
+      <c r="J5" s="136" t="str">
         <f>IFERROR(SUMIF(C$4:C5,"&gt;0",C$4:C5)/ABS(SUMIF(C$4:C5,"&lt;0",C$4:C5)),"")</f>
         <v/>
       </c>
-      <c r="K5" s="158" t="str">
+      <c r="K5" s="153" t="str">
         <f>IFERROR(AVERAGE($AG$4:AG5)/AK5*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="L5" s="141">
+      <c r="L5" s="136">
         <f>IFERROR(AVERAGE($AG$4:AG5)/_xlfn.STDEV.S($AG$4:AG5)*SQRT(12),"")</f>
         <v>33.276310483010022</v>
       </c>
-      <c r="M5" s="139">
+      <c r="M5" s="134">
         <f>MAX($C$4:C5)</f>
         <v>2.6599999999999957E-2</v>
       </c>
-      <c r="N5" s="139">
+      <c r="N5" s="134">
         <f>MIN($C$4:C5)</f>
         <v>2.3183323592441019E-2</v>
       </c>
-      <c r="O5" s="140">
+      <c r="O5" s="135">
         <f>IFERROR(AVERAGEIF($S$4:S5,"&gt;0",$C$4:C5)/AVERAGEIF($S$4:S5,"&gt;0",$S$4:S5),"")</f>
         <v>1.2531381706535767</v>
       </c>
-      <c r="P5" s="158" t="str">
+      <c r="P5" s="153" t="str">
         <f>IFERROR(AVERAGEIF($S$4:S5,"&lt;0",$C$4:C5)/AVERAGEIF($S$4:S5,"&lt;0",$S$4:S5),"-")</f>
         <v>-</v>
       </c>
-      <c r="Q5" s="143">
+      <c r="Q5" s="138">
         <f>IFERROR(SLOPE($C$4:C5,$S$4:S5),"")</f>
         <v>0.14423486072004843</v>
       </c>
-      <c r="R5" s="144">
-        <f>[2]Benchmarks!C5</f>
+      <c r="R5" s="139">
+        <f>[1]Benchmarks!C5</f>
         <v>442.46</v>
       </c>
-      <c r="S5" s="139">
+      <c r="S5" s="134">
         <f t="shared" ref="S5:S8" si="6">R5/R4-1</f>
         <v>8.0193192691484505E-3</v>
       </c>
-      <c r="T5" s="139">
+      <c r="T5" s="134">
         <f t="shared" ref="T5" si="7">((1+S5)*(1+T4))-1</f>
         <v>3.9981196380303397E-2</v>
       </c>
-      <c r="U5" s="140"/>
-      <c r="V5" s="142">
+      <c r="U5" s="135"/>
+      <c r="V5" s="137">
         <f t="shared" si="0"/>
         <v>0.25959430862843158</v>
       </c>
-      <c r="W5" s="139">
+      <c r="W5" s="134">
         <f>IFERROR(STDEV($S$4:S5),"")</f>
         <v>1.6750146565428777E-2</v>
       </c>
-      <c r="X5" s="141" t="str">
+      <c r="X5" s="136" t="str">
         <f>IFERROR(SUMIF(S$4:S5,"&gt;0",S$4:S5)/ABS(SUMIF(S$4:S5,"&lt;0",S$4:S5)),"")</f>
         <v/>
       </c>
-      <c r="Y5" s="158" t="str">
+      <c r="Y5" s="153" t="str">
         <f>IFERROR(AVERAGE($AV$4:AV5)/AZ5*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="Z5" s="141">
+      <c r="Z5" s="136">
         <f>IFERROR(AVERAGE($AV$4:AV5)/_xlfn.STDEV.S($AV$4:AV5)*SQRT(12),"")</f>
         <v>3.506533943562582</v>
       </c>
-      <c r="AA5" s="139">
+      <c r="AA5" s="134">
         <f>MAX($S$4:S5)</f>
         <v>3.1707603713714949E-2</v>
       </c>
-      <c r="AB5" s="139">
+      <c r="AB5" s="134">
         <f>MIN($S$4:S5)</f>
         <v>8.0193192691484505E-3</v>
       </c>
-      <c r="AC5" s="140"/>
-      <c r="AD5" s="139">
+      <c r="AC5" s="135"/>
+      <c r="AD5" s="134">
         <v>0</v>
       </c>
-      <c r="AE5" s="139">
+      <c r="AE5" s="134">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AF5" s="139">
+      <c r="AF5" s="134">
         <f t="shared" ref="AF5:AF8" si="8">((1+AE5)^(1/12))-1</f>
         <v>2.9516094330215292E-3</v>
       </c>
-      <c r="AG5" s="140">
+      <c r="AG5" s="135">
         <f>C5-AF5</f>
         <v>2.0231714159419489E-2</v>
       </c>
-      <c r="AH5" s="140">
+      <c r="AH5" s="135">
         <f>G5-(AF5*12)</f>
         <v>1.498068680374165E-2</v>
       </c>
-      <c r="AI5" s="139" t="str">
+      <c r="AI5" s="134" t="str">
         <f>IF(AG5&lt;0, AG5, "")</f>
         <v/>
       </c>
-      <c r="AJ5" s="139">
+      <c r="AJ5" s="134">
         <f t="shared" ref="AJ5:AJ8" si="9">IFERROR(AI5*AI5,0)</f>
         <v>0</v>
       </c>
-      <c r="AK5" s="139" cm="1">
+      <c r="AK5" s="134" cm="1">
         <f t="array" ref="AK5">IFERROR(SQRT(AVERAGE(IF($AG$4:AG5&lt;0,($AG$4:AG5)^2,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="AL5" s="139">
+      <c r="AL5" s="134">
         <f t="shared" ref="AL5:AL8" si="10">IFERROR(AK5*SQRT(12),"")</f>
         <v>0</v>
       </c>
-      <c r="AM5" s="139">
+      <c r="AM5" s="134">
         <f>IFERROR(AVERAGE($AG$4:AG5),"")</f>
         <v>2.1839319975472726E-2</v>
       </c>
-      <c r="AN5" s="139">
+      <c r="AN5" s="134">
         <f>IFERROR(_xlfn.STDEV.S($AG$4:AG5),"")</f>
         <v>2.2734979480123546E-3</v>
       </c>
-      <c r="AO5" s="141">
+      <c r="AO5" s="136">
         <f t="shared" ref="AO5:AO8" si="11">IFERROR(AM5/AN5*SQRT(12),"")</f>
         <v>33.276310483010022</v>
       </c>
-      <c r="AP5" s="139">
+      <c r="AP5" s="134">
         <f>IFERROR(CORREL($C$4:C5,$S$4:S5),"")</f>
         <v>1</v>
       </c>
-      <c r="AQ5" s="139">
+      <c r="AQ5" s="134">
         <f>IFERROR(RSQ($C$4:C5,$S$4:S5),"")</f>
         <v>1</v>
       </c>
-      <c r="AR5" s="139" cm="1">
+      <c r="AR5" s="134" cm="1">
         <f t="array" ref="AR5">IFERROR(_xlfn.STDEV.S($C$4:C5-$S$4:S5)*SQRT(12),"")</f>
         <v>4.9655095956371055E-2</v>
       </c>
-      <c r="AS5" s="139" cm="1">
+      <c r="AS5" s="134" cm="1">
         <f t="array" ref="AS5">IFERROR((AVERAGE($C$4:C5-$S$4:S5)*12)/(_xlfn.STDEV.S($C$4:C5-$S$4:S5)*SQRT(12)),"")</f>
         <v>1.2151502780395627</v>
       </c>
-      <c r="AT5" s="139"/>
-      <c r="AU5" s="140"/>
-      <c r="AV5" s="140">
+      <c r="AT5" s="134"/>
+      <c r="AU5" s="135"/>
+      <c r="AV5" s="135">
         <f>S5-AF5</f>
         <v>5.0677098361269213E-3</v>
       </c>
-      <c r="AW5" s="140">
+      <c r="AW5" s="135">
         <f>U5-(AF5*12)</f>
         <v>-3.5419313196258351E-2</v>
       </c>
-      <c r="AX5" s="139" t="str">
+      <c r="AX5" s="134" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AY5" s="139">
+      <c r="AY5" s="134">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AZ5" s="139" cm="1">
+      <c r="AZ5" s="134" cm="1">
         <f t="array" ref="AZ5">IFERROR(SQRT(AVERAGE(IF($AV$4:AV5&lt;0,($AV$4:AV5)^2,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="BA5" s="139">
+      <c r="BA5" s="134">
         <f t="shared" ref="BA5:BA8" si="12">IFERROR(AZ5*SQRT(12),"")</f>
         <v>0</v>
       </c>
-      <c r="BB5" s="139">
+      <c r="BB5" s="134">
         <f t="shared" si="3"/>
         <v>2.5681682983177548E-5</v>
       </c>
-      <c r="BC5" s="139">
+      <c r="BC5" s="134">
         <f>IFERROR(_xlfn.STDEV.S($AV$4:AV5),"")</f>
         <v>1.6607689456536116E-2</v>
       </c>
-      <c r="BD5" s="139">
+      <c r="BD5" s="134">
         <f t="shared" ref="BD5:BD8" si="13">IFERROR(BC5*SQRT(12),"")</f>
         <v>5.7530723870093017E-2</v>
       </c>
-      <c r="BE5" s="140"/>
-      <c r="BF5" s="145"/>
-      <c r="BG5" s="146"/>
-      <c r="BH5" s="147"/>
-      <c r="BI5" s="140">
+      <c r="BE5" s="135"/>
+      <c r="BF5" s="140"/>
+      <c r="BG5" s="141"/>
+      <c r="BH5" s="142"/>
+      <c r="BI5" s="135">
         <f>BN5/BK5</f>
         <v>0.63426789511730897</v>
       </c>
-      <c r="BJ5" s="140">
+      <c r="BJ5" s="135">
         <f>AVERAGE($BI$4:BI5)</f>
         <v>0.69968228508953856</v>
       </c>
-      <c r="BK5" s="148">
+      <c r="BK5" s="143">
         <v>16535083</v>
       </c>
-      <c r="BL5" s="148">
+      <c r="BL5" s="143">
         <v>6363581</v>
       </c>
-      <c r="BM5" s="148">
+      <c r="BM5" s="143">
         <v>1778665</v>
       </c>
-      <c r="BN5" s="148">
+      <c r="BN5" s="143">
         <v>10487672.289999999</v>
       </c>
-      <c r="BO5" s="149">
+      <c r="BO5" s="144">
         <f>BL5+BM5</f>
         <v>8142246</v>
       </c>
-      <c r="BP5" s="149">
+      <c r="BP5" s="144">
         <f>BL5-BM5</f>
         <v>4584916</v>
       </c>
-      <c r="BQ5" s="142">
+      <c r="BQ5" s="137">
         <f t="shared" ref="BQ5:BQ8" si="14">BL5/BK5</f>
         <v>0.38485328437722388</v>
       </c>
-      <c r="BR5" s="142">
+      <c r="BR5" s="137">
         <f t="shared" ref="BR5:BR8" si="15">-BM5/BK5</f>
         <v>-0.10756916067491164</v>
       </c>
-      <c r="BS5" s="142">
+      <c r="BS5" s="137">
         <f>BO5/BK5</f>
         <v>0.4924224450521355</v>
       </c>
-      <c r="BT5" s="142">
+      <c r="BT5" s="137">
         <f>BP5/BK5</f>
         <v>0.2772841237023122</v>
       </c>
-      <c r="BU5" s="142">
+      <c r="BU5" s="137">
         <f>AVERAGE($BS$4:BS5)</f>
         <v>0.36366282714968928</v>
       </c>
-      <c r="BV5" s="142">
+      <c r="BV5" s="137">
         <f>AVERAGE($BT$4:BT5)</f>
         <v>0.25223582229668418</v>
       </c>
-      <c r="BW5" s="150"/>
-      <c r="BX5" s="168" t="s">
+      <c r="BW5" s="145"/>
+      <c r="BX5" s="161" t="s">
         <v>279</v>
       </c>
-      <c r="BY5" s="152" t="e">
+      <c r="BY5" s="147" t="e">
         <f>BZ5/$BZ$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BZ5" s="169">
+      <c r="BZ5" s="162">
         <v>1399028.1584000001</v>
       </c>
       <c r="CB5" s="84" t="e">
         <f>"$1b-$10b (" &amp; TEXT(CC5,"0%") &amp; ")"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="CC5" s="154" t="e" cm="1">
+      <c r="CC5" s="149" t="e" cm="1">
         <f t="array" ref="CC5">SUMPRODUCT((CJ$3:CJ$15&gt;=1000000000)*(CJ$3:CJ$15&lt;10000000000)*CK$3:CK$15)</f>
         <v>#DIV/0!</v>
       </c>
@@ -9782,302 +9783,302 @@
       <c r="CF5" s="56" t="s">
         <v>282</v>
       </c>
-      <c r="CG5" s="155">
+      <c r="CG5" s="150">
         <v>5.1390241950458111E-2</v>
       </c>
-      <c r="CI5" s="156" cm="1">
+      <c r="CI5" s="151" cm="1">
         <f t="array" ref="CI5">_xll.BDP(CF5,"CUR_MKT_CAP","CURRENCY","AUD")</f>
         <v>2956829921952.3003</v>
       </c>
-      <c r="CJ5" s="156">
+      <c r="CJ5" s="151">
         <v>3149566246860</v>
       </c>
-      <c r="CK5" s="157" t="e">
+      <c r="CK5" s="152" t="e">
         <f>CG5/$CG$16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:134" s="56" customFormat="1" ht="15.5">
-      <c r="A6" s="137">
+      <c r="A6" s="132">
         <v>45930</v>
       </c>
-      <c r="B6" s="138">
+      <c r="B6" s="133">
         <v>1.085396</v>
       </c>
-      <c r="C6" s="139">
+      <c r="C6" s="134">
         <f>B6/B5-1</f>
         <v>3.3316831683168235E-2</v>
       </c>
-      <c r="D6" s="139">
+      <c r="D6" s="134">
         <f>((1+C6)*(1+D5))-1</f>
         <v>8.5395999999999805E-2</v>
       </c>
-      <c r="E6" s="139">
+      <c r="E6" s="134">
         <f t="shared" ref="E6:E8" si="16">((1+C6)*(1+C5)*(1+C4)-1)</f>
         <v>8.5395999999999805E-2</v>
       </c>
-      <c r="F6" s="139">
+      <c r="F6" s="134">
         <f>D6</f>
         <v>8.5395999999999805E-2</v>
       </c>
-      <c r="G6" s="139">
+      <c r="G6" s="134">
         <f>D6</f>
         <v>8.5395999999999805E-2</v>
       </c>
-      <c r="H6" s="140">
+      <c r="H6" s="135">
         <f>((1+D6)^(365/(_xlfn.DAYS(A6,"1/07/2025"))))-1</f>
         <v>0.38913337687433036</v>
       </c>
-      <c r="I6" s="139">
+      <c r="I6" s="134">
         <f>IFERROR(_xlfn.STDEV.S($C$4:C6)*SQRT(12),"")</f>
         <v>1.785931083546154E-2</v>
       </c>
-      <c r="J6" s="141" t="str">
+      <c r="J6" s="136" t="str">
         <f>IFERROR(SUMIF(C$4:C6,"&gt;0",C$4:C6)/ABS(SUMIF(C$4:C6,"&lt;0",C$4:C6)),"")</f>
         <v/>
       </c>
-      <c r="K6" s="158" t="str">
+      <c r="K6" s="153" t="str">
         <f>IFERROR(AVERAGE($AG$4:AG6)/AK6*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="L6" s="141">
+      <c r="L6" s="136">
         <f>IFERROR(AVERAGE($AG$4:AG6)/_xlfn.STDEV.S($AG$4:AG6)*SQRT(12),"")</f>
         <v>16.510935992589282</v>
       </c>
-      <c r="M6" s="139">
+      <c r="M6" s="134">
         <f>MAX($C$4:C6)</f>
         <v>3.3316831683168235E-2</v>
       </c>
-      <c r="N6" s="139">
+      <c r="N6" s="134">
         <f>MIN($C$4:C6)</f>
         <v>2.3183323592441019E-2</v>
       </c>
-      <c r="O6" s="140">
+      <c r="O6" s="135">
         <f>IFERROR(AVERAGEIF($S$4:S6,"&gt;0",$C$4:C6)/AVERAGEIF($S$4:S6,"&gt;0",$S$4:S6),"")</f>
         <v>1.3175095137736863</v>
       </c>
-      <c r="P6" s="158" t="str">
+      <c r="P6" s="153" t="str">
         <f>IFERROR(AVERAGEIF($S$4:S6,"&lt;0",$C$4:C6)/AVERAGEIF($S$4:S6,"&lt;0",$S$4:S6),"-")</f>
         <v>-</v>
       </c>
-      <c r="Q6" s="143">
+      <c r="Q6" s="138">
         <f>IFERROR(SLOPE($C$4:C6,$S$4:S6),"")</f>
         <v>0.20797204045248729</v>
       </c>
-      <c r="R6" s="144">
-        <f>[2]Benchmarks!C6</f>
+      <c r="R6" s="139">
+        <f>[1]Benchmarks!C6</f>
         <v>452.79</v>
       </c>
-      <c r="S6" s="139">
+      <c r="S6" s="134">
         <f t="shared" si="6"/>
         <v>2.334674320842578E-2</v>
       </c>
-      <c r="T6" s="139">
+      <c r="T6" s="134">
         <f>((1+S6)*(1+T5))-1</f>
         <v>6.4261370313785759E-2</v>
       </c>
-      <c r="U6" s="140"/>
-      <c r="V6" s="142">
+      <c r="U6" s="135"/>
+      <c r="V6" s="137">
         <f t="shared" si="0"/>
         <v>0.28029834869624226</v>
       </c>
-      <c r="W6" s="139">
+      <c r="W6" s="134">
         <f>IFERROR(STDEV($S$4:S6),"")</f>
         <v>1.2013663977113219E-2</v>
       </c>
-      <c r="X6" s="141" t="str">
+      <c r="X6" s="136" t="str">
         <f>IFERROR(SUMIF(S$4:S6,"&gt;0",S$4:S6)/ABS(SUMIF(S$4:S6,"&lt;0",S$4:S6)),"")</f>
         <v/>
       </c>
-      <c r="Y6" s="158" t="str">
+      <c r="Y6" s="153" t="str">
         <f>IFERROR(AVERAGE($AV$4:AV6)/AZ6*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="Z6" s="141">
+      <c r="Z6" s="136">
         <f>IFERROR(AVERAGE($AV$4:AV6)/_xlfn.STDEV.S($AV$4:AV6)*SQRT(12),"")</f>
         <v>5.2308134019704857</v>
       </c>
-      <c r="AA6" s="139">
+      <c r="AA6" s="134">
         <f>MAX($S$4:S6)</f>
         <v>3.1707603713714949E-2</v>
       </c>
-      <c r="AB6" s="139">
+      <c r="AB6" s="134">
         <f>MIN($S$4:S6)</f>
         <v>8.0193192691484505E-3</v>
       </c>
-      <c r="AC6" s="140"/>
-      <c r="AD6" s="139">
+      <c r="AC6" s="135"/>
+      <c r="AD6" s="134">
         <v>0</v>
       </c>
-      <c r="AE6" s="139">
+      <c r="AE6" s="134">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AF6" s="139">
+      <c r="AF6" s="134">
         <f t="shared" si="8"/>
         <v>2.9516094330215292E-3</v>
       </c>
-      <c r="AG6" s="140">
+      <c r="AG6" s="135">
         <f>C6-AF6</f>
         <v>3.0365222250146706E-2</v>
       </c>
-      <c r="AH6" s="140">
+      <c r="AH6" s="135">
         <f>G6-(AF6*12)</f>
         <v>4.9976686803741455E-2</v>
       </c>
-      <c r="AI6" s="139" t="str">
+      <c r="AI6" s="134" t="str">
         <f t="shared" ref="AI6:AI8" si="17">IF(AG6&lt;0, AG6, "")</f>
         <v/>
       </c>
-      <c r="AJ6" s="139">
+      <c r="AJ6" s="134">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AK6" s="139" cm="1">
+      <c r="AK6" s="134" cm="1">
         <f t="array" ref="AK6">IFERROR(SQRT(AVERAGE(IF($AG$4:AG6&lt;0,($AG$4:AG6)^2,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="AL6" s="139">
+      <c r="AL6" s="134">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AM6" s="139">
+      <c r="AM6" s="134">
         <f>IFERROR(AVERAGE($AG$4:AG6),"")</f>
         <v>2.4681287400364054E-2</v>
       </c>
-      <c r="AN6" s="139">
+      <c r="AN6" s="134">
         <f>IFERROR(_xlfn.STDEV.S($AG$4:AG6),"")</f>
         <v>5.178294409575273E-3</v>
       </c>
-      <c r="AO6" s="141">
+      <c r="AO6" s="136">
         <f t="shared" si="11"/>
         <v>16.510935992589282</v>
       </c>
-      <c r="AP6" s="139">
+      <c r="AP6" s="134">
         <f>IFERROR(CORREL($C$4:C6,$S$4:S6),"")</f>
         <v>0.48462560954436296</v>
       </c>
-      <c r="AQ6" s="139">
+      <c r="AQ6" s="134">
         <f>IFERROR(RSQ($C$4:C6,$S$4:S6),"")</f>
         <v>0.23486198142624545</v>
       </c>
-      <c r="AR6" s="139" cm="1">
+      <c r="AR6" s="134" cm="1">
         <f t="array" ref="AR6">IFERROR(_xlfn.STDEV.S($C$4:C6-$S$4:S6)*SQRT(12),"")</f>
         <v>3.6476064918731579E-2</v>
       </c>
-      <c r="AS6" s="139" cm="1">
+      <c r="AS6" s="134" cm="1">
         <f t="array" ref="AS6">IFERROR((AVERAGE($C$4:C6-$S$4:S6)*12)/(_xlfn.STDEV.S($C$4:C6-$S$4:S6)*SQRT(12)),"")</f>
         <v>2.1961238558971656</v>
       </c>
-      <c r="AT6" s="139"/>
-      <c r="AU6" s="140"/>
-      <c r="AV6" s="140">
+      <c r="AT6" s="134"/>
+      <c r="AU6" s="135"/>
+      <c r="AV6" s="135">
         <f>S6-AF6</f>
         <v>2.0395133775404251E-2</v>
       </c>
-      <c r="AW6" s="140">
+      <c r="AW6" s="135">
         <f>U6-(AF6*12)</f>
         <v>-3.5419313196258351E-2</v>
       </c>
-      <c r="AX6" s="139" t="str">
+      <c r="AX6" s="134" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AY6" s="139">
+      <c r="AY6" s="134">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AZ6" s="139" cm="1">
+      <c r="AZ6" s="134" cm="1">
         <f t="array" ref="AZ6">IFERROR(SQRT(AVERAGE(IF($AV$4:AV6&lt;0,($AV$4:AV6)^2,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="BA6" s="139">
+      <c r="BA6" s="134">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="BB6" s="139">
+      <c r="BB6" s="134">
         <f t="shared" si="3"/>
         <v>4.1596148171663523E-4</v>
       </c>
-      <c r="BC6" s="139">
+      <c r="BC6" s="134">
         <f>IFERROR(_xlfn.STDEV.S($AV$4:AV6),"")</f>
         <v>1.1924319417754984E-2</v>
       </c>
-      <c r="BD6" s="139">
+      <c r="BD6" s="134">
         <f t="shared" si="13"/>
         <v>4.1307054154463528E-2</v>
       </c>
-      <c r="BE6" s="140"/>
-      <c r="BF6" s="145"/>
-      <c r="BG6" s="146"/>
-      <c r="BH6" s="147"/>
-      <c r="BI6" s="140">
+      <c r="BE6" s="135"/>
+      <c r="BF6" s="140"/>
+      <c r="BG6" s="141"/>
+      <c r="BH6" s="142"/>
+      <c r="BI6" s="135">
         <f>BN6/BK6</f>
         <v>0.64644687379893429</v>
       </c>
-      <c r="BJ6" s="140">
+      <c r="BJ6" s="135">
         <f>AVERAGE($BI$4:BI6)</f>
         <v>0.68193714799267047</v>
       </c>
-      <c r="BK6" s="148">
+      <c r="BK6" s="143">
         <v>17156638</v>
       </c>
-      <c r="BL6" s="148">
+      <c r="BL6" s="143">
         <v>7772590</v>
       </c>
-      <c r="BM6" s="148">
+      <c r="BM6" s="143">
         <v>4351270</v>
       </c>
-      <c r="BN6" s="148">
+      <c r="BN6" s="143">
         <v>11090855</v>
       </c>
-      <c r="BO6" s="149">
+      <c r="BO6" s="144">
         <f>BL6+BM6</f>
         <v>12123860</v>
       </c>
-      <c r="BP6" s="149">
+      <c r="BP6" s="144">
         <f>BL6-BM6</f>
         <v>3421320</v>
       </c>
-      <c r="BQ6" s="142">
+      <c r="BQ6" s="137">
         <f t="shared" si="14"/>
         <v>0.45303689452444007</v>
       </c>
-      <c r="BR6" s="142">
+      <c r="BR6" s="137">
         <f t="shared" si="15"/>
         <v>-0.25362020227972404</v>
       </c>
-      <c r="BS6" s="142">
+      <c r="BS6" s="137">
         <f>BO6/BK6</f>
         <v>0.70665709680416411</v>
       </c>
-      <c r="BT6" s="142">
+      <c r="BT6" s="137">
         <f>BP6/BK6</f>
         <v>0.199416692244716</v>
       </c>
-      <c r="BU6" s="142">
+      <c r="BU6" s="137">
         <f>AVERAGE($BS$4:BS6)</f>
         <v>0.4779942503678476</v>
       </c>
-      <c r="BV6" s="142">
+      <c r="BV6" s="137">
         <f>AVERAGE($BT$4:BT6)</f>
         <v>0.2346294456126948</v>
       </c>
-      <c r="BW6" s="150"/>
-      <c r="BX6" s="165" t="s">
+      <c r="BW6" s="145"/>
+      <c r="BX6" s="158" t="s">
         <v>96</v>
       </c>
-      <c r="BY6" s="152" t="e">
+      <c r="BY6" s="147" t="e">
         <f>BZ6/$BZ$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BZ6" s="169">
+      <c r="BZ6" s="162">
         <v>1250122.2307104699</v>
       </c>
       <c r="CB6" s="84" t="e">
         <f>"$500m-$1b (" &amp; TEXT(CC6,"0%") &amp; ")"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="CC6" s="154" t="e" cm="1">
+      <c r="CC6" s="149" t="e" cm="1">
         <f t="array" ref="CC6">SUMPRODUCT((CJ$3:CJ$15&gt;=500000000)*(CJ$3:CJ$15&lt;1000000000)*CK$3:CK$15)</f>
         <v>#DIV/0!</v>
       </c>
@@ -10090,301 +10091,301 @@
       <c r="CF6" s="56" t="s">
         <v>284</v>
       </c>
-      <c r="CG6" s="155">
+      <c r="CG6" s="150">
         <v>4.7334742913622177E-2</v>
       </c>
-      <c r="CI6" s="156" cm="1">
+      <c r="CI6" s="151" cm="1">
         <f t="array" ref="CI6">_xll.BDP(CF6,"CUR_MKT_CAP","CURRENCY","AUD")</f>
         <v>51088575.100000001</v>
       </c>
-      <c r="CJ6" s="156">
+      <c r="CJ6" s="151">
         <v>42689751.085000001</v>
       </c>
-      <c r="CK6" s="157" t="e">
+      <c r="CK6" s="152" t="e">
         <f>CG6/$CG$16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:134" s="56" customFormat="1" ht="15.5">
-      <c r="A7" s="137">
+      <c r="A7" s="132">
         <v>45961</v>
       </c>
-      <c r="B7" s="138">
-        <f>[1]Monthly!$G$41</f>
+      <c r="B7" s="133">
+        <f>[2]Monthly!$G$41</f>
         <v>1.1200237411717677</v>
       </c>
-      <c r="C7" s="139">
+      <c r="C7" s="134">
         <f>B7/B6-1</f>
         <v>3.1903324843437497E-2</v>
       </c>
-      <c r="D7" s="139">
+      <c r="D7" s="134">
         <f>((1+C7)*(1+D6))-1</f>
         <v>0.12002374117176751</v>
       </c>
-      <c r="E7" s="139">
+      <c r="E7" s="134">
         <f t="shared" si="16"/>
         <v>9.1003059781577633E-2</v>
       </c>
-      <c r="F7" s="139">
+      <c r="F7" s="134">
         <f>D7</f>
         <v>0.12002374117176751</v>
       </c>
-      <c r="G7" s="139">
+      <c r="G7" s="134">
         <f>D7</f>
         <v>0.12002374117176751</v>
       </c>
-      <c r="H7" s="140">
+      <c r="H7" s="135">
         <f>((1+D7)^(365/(_xlfn.DAYS(A7,"1/07/2025"))))-1</f>
         <v>0.40371255294551722</v>
       </c>
-      <c r="I7" s="139">
+      <c r="I7" s="134">
         <f>IFERROR(_xlfn.STDEV.S($C$4:C7)*SQRT(12),"")</f>
         <v>1.6298440709380285E-2</v>
       </c>
-      <c r="J7" s="141" t="str">
+      <c r="J7" s="136" t="str">
         <f>IFERROR(SUMIF(C$4:C7,"&gt;0",C$4:C7)/ABS(SUMIF(C$4:C7,"&lt;0",C$4:C7)),"")</f>
         <v/>
       </c>
-      <c r="K7" s="158" t="str">
+      <c r="K7" s="153" t="str">
         <f>IFERROR(AVERAGE($AG$4:AG7)/AK7*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="L7" s="141">
+      <c r="L7" s="136">
         <f>IFERROR(AVERAGE($AG$4:AG7)/_xlfn.STDEV.S($AG$4:AG7)*SQRT(12),"")</f>
         <v>18.831291180530624</v>
       </c>
-      <c r="M7" s="139">
+      <c r="M7" s="134">
         <f>MAX($C$4:C7)</f>
         <v>3.3316831683168235E-2</v>
       </c>
-      <c r="N7" s="139">
+      <c r="N7" s="134">
         <f>MIN($C$4:C7)</f>
         <v>2.3183323592441019E-2</v>
       </c>
-      <c r="O7" s="140">
+      <c r="O7" s="135">
         <f>IFERROR(AVERAGEIF($S$4:S7,"&gt;0",$C$4:C7)/AVERAGEIF($S$4:S7,"&gt;0",$S$4:S7),"")</f>
         <v>1.1722974145510086</v>
       </c>
-      <c r="P7" s="158" t="str">
+      <c r="P7" s="153" t="str">
         <f>IFERROR(AVERAGEIF($S$4:S7,"&lt;0",$C$4:C7)/AVERAGEIF($S$4:S7,"&lt;0",$S$4:S7),"-")</f>
         <v>-</v>
       </c>
-      <c r="Q7" s="143">
+      <c r="Q7" s="138">
         <f>IFERROR(SLOPE($C$4:C7,$S$4:S7),"")</f>
         <v>0.23909151636201728</v>
       </c>
-      <c r="R7" s="144">
-        <f>[2]Benchmarks!C7</f>
+      <c r="R7" s="139">
+        <f>[1]Benchmarks!C7</f>
         <v>468.65</v>
       </c>
-      <c r="S7" s="139">
+      <c r="S7" s="134">
         <f t="shared" si="6"/>
         <v>3.5027275337352837E-2</v>
       </c>
-      <c r="T7" s="139">
+      <c r="T7" s="134">
         <f>((1+S7)*(1+T6))-1</f>
         <v>0.10153954636267515</v>
       </c>
-      <c r="U7" s="140"/>
-      <c r="V7" s="142">
+      <c r="U7" s="135"/>
+      <c r="V7" s="137">
         <f t="shared" si="0"/>
         <v>0.3323993845492037</v>
       </c>
-      <c r="W7" s="139">
+      <c r="W7" s="134">
         <f>IFERROR(STDEV($S$4:S7),"")</f>
         <v>1.2051464207084511E-2</v>
       </c>
-      <c r="X7" s="141" t="str">
+      <c r="X7" s="136" t="str">
         <f>IFERROR(SUMIF(S$4:S7,"&gt;0",S$4:S7)/ABS(SUMIF(S$4:S7,"&lt;0",S$4:S7)),"")</f>
         <v/>
       </c>
-      <c r="Y7" s="158" t="str">
+      <c r="Y7" s="153" t="str">
         <f>IFERROR(AVERAGE($AV$4:AV7)/AZ7*SQRT(12),"")</f>
         <v/>
       </c>
-      <c r="Z7" s="141">
+      <c r="Z7" s="136">
         <f>IFERROR(AVERAGE($AV$4:AV7)/_xlfn.STDEV.S($AV$4:AV7)*SQRT(12),"")</f>
         <v>6.2071276417102865</v>
       </c>
-      <c r="AA7" s="139">
+      <c r="AA7" s="134">
         <f>MAX($S$4:S7)</f>
         <v>3.5027275337352837E-2</v>
       </c>
-      <c r="AB7" s="139">
+      <c r="AB7" s="134">
         <f>MIN($S$4:S7)</f>
         <v>8.0193192691484505E-3</v>
       </c>
-      <c r="AC7" s="140"/>
-      <c r="AD7" s="139">
+      <c r="AC7" s="135"/>
+      <c r="AD7" s="134">
         <v>0</v>
       </c>
-      <c r="AE7" s="139">
+      <c r="AE7" s="134">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AF7" s="139">
+      <c r="AF7" s="134">
         <f t="shared" si="8"/>
         <v>2.9516094330215292E-3</v>
       </c>
-      <c r="AG7" s="140">
+      <c r="AG7" s="135">
         <f>C7-AF7</f>
         <v>2.8951715410415968E-2</v>
       </c>
-      <c r="AH7" s="140">
+      <c r="AH7" s="135">
         <f>G7-(AF7*12)</f>
         <v>8.4604427975509156E-2</v>
       </c>
-      <c r="AI7" s="139" t="str">
+      <c r="AI7" s="134" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AJ7" s="139">
+      <c r="AJ7" s="134">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AK7" s="139" cm="1">
+      <c r="AK7" s="134" cm="1">
         <f t="array" ref="AK7">IFERROR(SQRT(AVERAGE(IF($AG$4:AG7&lt;0,($AG$4:AG7)^2,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="AL7" s="139">
+      <c r="AL7" s="134">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AM7" s="139">
+      <c r="AM7" s="134">
         <f>IFERROR(AVERAGE($AG$4:AG7),"")</f>
         <v>2.5748894402877032E-2</v>
       </c>
-      <c r="AN7" s="139">
+      <c r="AN7" s="134">
         <f>IFERROR(_xlfn.STDEV.S($AG$4:AG7),"")</f>
         <v>4.7366261736336472E-3</v>
       </c>
-      <c r="AO7" s="141">
+      <c r="AO7" s="136">
         <f t="shared" si="11"/>
         <v>18.831291180530624</v>
       </c>
-      <c r="AP7" s="139">
+      <c r="AP7" s="134">
         <f>IFERROR(CORREL($C$4:C7,$S$4:S7),"")</f>
         <v>0.61241884731549301</v>
       </c>
-      <c r="AQ7" s="139">
+      <c r="AQ7" s="134">
         <f>IFERROR(RSQ($C$4:C7,$S$4:S7),"")</f>
         <v>0.37505684454723687</v>
       </c>
-      <c r="AR7" s="139" cm="1">
+      <c r="AR7" s="134" cm="1">
         <f t="array" ref="AR7">IFERROR(_xlfn.STDEV.S($C$4:C7-$S$4:S7)*SQRT(12),"")</f>
         <v>3.4279581152387911E-2</v>
       </c>
-      <c r="AS7" s="139" cm="1">
+      <c r="AS7" s="134" cm="1">
         <f t="array" ref="AS7">IFERROR((AVERAGE($C$4:C7-$S$4:S7)*12)/(_xlfn.STDEV.S($C$4:C7-$S$4:S7)*SQRT(12)),"")</f>
         <v>1.4792367370475235</v>
       </c>
-      <c r="AT7" s="139"/>
-      <c r="AU7" s="140"/>
-      <c r="AV7" s="140">
+      <c r="AT7" s="134"/>
+      <c r="AU7" s="135"/>
+      <c r="AV7" s="135">
         <f>S7-AF7</f>
         <v>3.2075665904331307E-2</v>
       </c>
-      <c r="AW7" s="140">
+      <c r="AW7" s="135">
         <f>U7-(AF7*12)</f>
         <v>-3.5419313196258351E-2</v>
       </c>
-      <c r="AX7" s="139" t="str">
+      <c r="AX7" s="134" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AY7" s="139">
+      <c r="AY7" s="134">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AZ7" s="139" cm="1">
+      <c r="AZ7" s="134" cm="1">
         <f t="array" ref="AZ7">IFERROR(SQRT(AVERAGE(IF($AV$4:AV7&lt;0,($AV$4:AV7)^2,0))),"")</f>
         <v>0</v>
       </c>
-      <c r="BA7" s="139">
+      <c r="BA7" s="134">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="BB7" s="139">
+      <c r="BB7" s="134">
         <f t="shared" si="3"/>
         <v>1.0288483432062819E-3</v>
       </c>
-      <c r="BC7" s="139">
+      <c r="BC7" s="134">
         <f>IFERROR(_xlfn.STDEV.S($AV$4:AV7),"")</f>
         <v>1.201179727322909E-2</v>
       </c>
-      <c r="BD7" s="139">
+      <c r="BD7" s="134">
         <f t="shared" si="13"/>
         <v>4.1610086334900161E-2</v>
       </c>
-      <c r="BE7" s="140"/>
-      <c r="BF7" s="145"/>
-      <c r="BG7" s="146"/>
-      <c r="BH7" s="147"/>
-      <c r="BI7" s="140">
+      <c r="BE7" s="135"/>
+      <c r="BF7" s="140"/>
+      <c r="BG7" s="141"/>
+      <c r="BH7" s="142"/>
+      <c r="BI7" s="135">
         <f>BN7/BK7</f>
         <v>0.77467030468394726</v>
       </c>
-      <c r="BJ7" s="140">
+      <c r="BJ7" s="135">
         <f>AVERAGE($BI$4:BI7)</f>
         <v>0.70512043716548967</v>
       </c>
-      <c r="BK7" s="148">
+      <c r="BK7" s="143">
         <v>21990000</v>
       </c>
-      <c r="BL7" s="148">
+      <c r="BL7" s="143">
         <v>6370000</v>
       </c>
-      <c r="BM7" s="148">
+      <c r="BM7" s="143">
         <v>4171000</v>
       </c>
-      <c r="BN7" s="148">
+      <c r="BN7" s="143">
         <v>17035000</v>
       </c>
-      <c r="BO7" s="149">
+      <c r="BO7" s="144">
         <v>10574000</v>
       </c>
-      <c r="BP7" s="149">
+      <c r="BP7" s="144">
         <v>2231000</v>
       </c>
-      <c r="BQ7" s="142">
+      <c r="BQ7" s="137">
         <f t="shared" si="14"/>
         <v>0.28967712596634831</v>
       </c>
-      <c r="BR7" s="142">
+      <c r="BR7" s="137">
         <f t="shared" si="15"/>
         <v>-0.18967712596634834</v>
       </c>
-      <c r="BS7" s="142">
+      <c r="BS7" s="137">
         <f>BO7/BK7</f>
         <v>0.48085493406093677</v>
       </c>
-      <c r="BT7" s="142">
+      <c r="BT7" s="137">
         <f>BP7/BK7</f>
         <v>0.10145520691223284</v>
       </c>
-      <c r="BU7" s="142">
+      <c r="BU7" s="137">
         <f>AVERAGE($BS$4:BS7)</f>
         <v>0.47870942129111987</v>
       </c>
-      <c r="BV7" s="142">
+      <c r="BV7" s="137">
         <f>AVERAGE($BT$4:BT7)</f>
         <v>0.20133588593757931</v>
       </c>
-      <c r="BW7" s="150"/>
-      <c r="BX7" s="151" t="s">
+      <c r="BW7" s="145"/>
+      <c r="BX7" s="146" t="s">
         <v>247</v>
       </c>
-      <c r="BY7" s="152" t="e">
+      <c r="BY7" s="147" t="e">
         <f>BZ7/$BZ$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BZ7" s="153">
+      <c r="BZ7" s="148">
         <v>1006416.30252</v>
       </c>
       <c r="CB7" s="84" t="e">
         <f>"$500m-$1b (" &amp; TEXT(CC7,"0%") &amp; ")"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="CC7" s="154" t="e" cm="1">
+      <c r="CC7" s="149" t="e" cm="1">
         <f t="array" ref="CC7">SUMPRODUCT((CJ$3:CJ$15&gt;=500000000)*(CJ$3:CJ$15&lt;1000000000)*CK$3:CK$15)</f>
         <v>#DIV/0!</v>
       </c>
@@ -10397,301 +10398,301 @@
       <c r="CF7" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="CG7" s="155">
+      <c r="CG7" s="150">
         <v>4.7334742913622177E-2</v>
       </c>
-      <c r="CI7" s="156" cm="1">
+      <c r="CI7" s="151" cm="1">
         <f t="array" ref="CI7">_xll.BDP(CF7,"CUR_MKT_CAP","CURRENCY","AUD")</f>
         <v>41020148249.550003</v>
       </c>
-      <c r="CJ7" s="156">
+      <c r="CJ7" s="151">
         <v>34799002284.599998</v>
       </c>
-      <c r="CK7" s="157" t="e">
+      <c r="CK7" s="152" t="e">
         <f t="shared" ref="CK7:CK8" si="18">CG7/$CG$16</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:134" s="56" customFormat="1" ht="15.5">
-      <c r="A8" s="137">
+      <c r="A8" s="132">
         <v>45991</v>
       </c>
-      <c r="B8" s="138">
-        <f>[1]Monthly!$H$41</f>
+      <c r="B8" s="133">
+        <f>[2]Monthly!$H$41</f>
         <v>1.1169995713674072</v>
       </c>
-      <c r="C8" s="139">
+      <c r="C8" s="134">
         <f>B8/B7-1</f>
         <v>-2.7000943758537232E-3</v>
       </c>
-      <c r="D8" s="139">
+      <c r="D8" s="134">
         <f>((1+C8)*(1+D7))-1</f>
         <v>0.11699957136740702</v>
       </c>
-      <c r="E8" s="139">
+      <c r="E8" s="134">
         <f t="shared" si="16"/>
         <v>6.340400929875023E-2</v>
       </c>
-      <c r="F8" s="139">
+      <c r="F8" s="134">
         <f>D8</f>
         <v>0.11699957136740702</v>
       </c>
-      <c r="G8" s="139">
+      <c r="G8" s="134">
         <f>D8</f>
         <v>0.11699957136740702</v>
       </c>
-      <c r="H8" s="140">
+      <c r="H8" s="135">
         <f>((1+D8)^(365/(_xlfn.DAYS(A8,"1/07/2025"))))-1</f>
         <v>0.30433888942018061</v>
       </c>
-      <c r="I8" s="139">
+      <c r="I8" s="134">
         <f>IFERROR(_xlfn.STDEV.S($C$4:C8)*SQRT(12),"")</f>
         <v>5.0726925454552985E-2</v>
       </c>
-      <c r="J8" s="141">
+      <c r="J8" s="136">
         <f>IFERROR(SUMIF(C$4:C8,"&gt;0",C$4:C8)/ABS(SUMIF(C$4:C8,"&lt;0",C$4:C8)),"")</f>
         <v>42.59239275022918</v>
       </c>
-      <c r="K8" s="141">
+      <c r="K8" s="136">
         <f>IFERROR(AVERAGE($AG$4:AG8)/AK8*SQRT(12),"")</f>
         <v>26.683012050339038</v>
       </c>
-      <c r="L8" s="141">
+      <c r="L8" s="136">
         <f>IFERROR(AVERAGE($AG$4:AG8)/_xlfn.STDEV.S($AG$4:AG8)*SQRT(12),"")</f>
         <v>4.6099449429478758</v>
       </c>
-      <c r="M8" s="139">
+      <c r="M8" s="134">
         <f>MAX($C$4:C8)</f>
         <v>3.3316831683168235E-2</v>
       </c>
-      <c r="N8" s="139">
+      <c r="N8" s="134">
         <f>MIN($C$4:C8)</f>
         <v>-2.7000943758537232E-3</v>
       </c>
-      <c r="O8" s="140">
+      <c r="O8" s="135">
         <f>IFERROR(AVERAGEIF($S$4:S8,"&gt;0",$C$4:C8)/AVERAGEIF($S$4:S8,"&gt;0",$S$4:S8),"")</f>
         <v>1.1722974145510086</v>
       </c>
-      <c r="P8" s="142">
+      <c r="P8" s="137">
         <f>IFERROR(AVERAGEIF($S$4:S8,"&lt;0",$C$4:C8)/AVERAGEIF($S$4:S8,"&lt;0",$S$4:S8),"-")</f>
         <v>1.4379536695952804</v>
       </c>
-      <c r="Q8" s="143">
+      <c r="Q8" s="138">
         <f>IFERROR(SLOPE($C$4:C8,$S$4:S8),"")</f>
         <v>0.77359491498646449</v>
       </c>
-      <c r="R8" s="144">
-        <f>[2]Benchmarks!C8</f>
+      <c r="R8" s="139">
+        <f>[1]Benchmarks!C8</f>
         <v>467.77</v>
       </c>
-      <c r="S8" s="139">
+      <c r="S8" s="134">
         <f t="shared" si="6"/>
         <v>-1.8777339165688689E-3</v>
       </c>
-      <c r="T8" s="139">
+      <c r="T8" s="134">
         <f>((1+S8)*(1+T7))-1</f>
         <v>9.9471148196027981E-2</v>
       </c>
-      <c r="U8" s="140"/>
-      <c r="V8" s="142">
+      <c r="U8" s="135"/>
+      <c r="V8" s="137">
         <f t="shared" si="0"/>
         <v>0.25385992970414772</v>
       </c>
-      <c r="W8" s="139">
+      <c r="W8" s="134">
         <f>IFERROR(STDEV($S$4:S8),"")</f>
         <v>1.5759178268834592E-2</v>
       </c>
-      <c r="X8" s="141">
+      <c r="X8" s="136">
         <f>IFERROR(SUMIF(S$4:S8,"&gt;0",S$4:S8)/ABS(SUMIF(S$4:S8,"&lt;0",S$4:S8)),"")</f>
         <v>52.244325281134159</v>
       </c>
-      <c r="Y8" s="141">
+      <c r="Y8" s="136">
         <f>IFERROR(AVERAGE($AV$4:AV8)/AZ8*SQRT(12),"")</f>
         <v>26.068383811536769</v>
       </c>
-      <c r="Z8" s="141">
+      <c r="Z8" s="136">
         <f>IFERROR(AVERAGE($AV$4:AV8)/_xlfn.STDEV.S($AV$4:AV8)*SQRT(12),"")</f>
         <v>3.5815989517710856</v>
       </c>
-      <c r="AA8" s="139">
+      <c r="AA8" s="134">
         <f>MAX($S$4:S8)</f>
         <v>3.5027275337352837E-2</v>
       </c>
-      <c r="AB8" s="139">
+      <c r="AB8" s="134">
         <f>MIN($S$4:S8)</f>
         <v>-1.8777339165688689E-3</v>
       </c>
-      <c r="AC8" s="140"/>
-      <c r="AD8" s="139">
+      <c r="AC8" s="135"/>
+      <c r="AD8" s="134">
         <v>0</v>
       </c>
-      <c r="AE8" s="139">
+      <c r="AE8" s="134">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AF8" s="139">
+      <c r="AF8" s="134">
         <f t="shared" si="8"/>
         <v>2.9516094330215292E-3</v>
       </c>
-      <c r="AG8" s="140">
+      <c r="AG8" s="135">
         <f>C8-AF8</f>
         <v>-5.6517038088752525E-3</v>
       </c>
-      <c r="AH8" s="140">
+      <c r="AH8" s="135">
         <f>G8-(AF8*12)</f>
         <v>8.1580258171148667E-2</v>
       </c>
-      <c r="AI8" s="139">
+      <c r="AI8" s="134">
         <f t="shared" si="17"/>
         <v>-5.6517038088752525E-3</v>
       </c>
-      <c r="AJ8" s="139">
+      <c r="AJ8" s="134">
         <f t="shared" si="9"/>
         <v>3.194175594325504E-5</v>
       </c>
-      <c r="AK8" s="139" cm="1">
+      <c r="AK8" s="134" cm="1">
         <f t="array" ref="AK8">IFERROR(SQRT(AVERAGE(IF($AG$4:AG8&lt;0,($AG$4:AG8)^2,0))),"")</f>
         <v>2.527518781067909E-3</v>
       </c>
-      <c r="AL8" s="139">
+      <c r="AL8" s="134">
         <f t="shared" si="10"/>
         <v>8.7555818917883516E-3</v>
       </c>
-      <c r="AM8" s="139">
+      <c r="AM8" s="134">
         <f>IFERROR(AVERAGE($AG$4:AG8),"")</f>
         <v>1.9468774760526573E-2</v>
       </c>
-      <c r="AN8" s="139">
+      <c r="AN8" s="134">
         <f>IFERROR(_xlfn.STDEV.S($AG$4:AG8),"")</f>
         <v>1.4629635478806153E-2</v>
       </c>
-      <c r="AO8" s="141">
+      <c r="AO8" s="136">
         <f t="shared" si="11"/>
         <v>4.6099449429478758</v>
       </c>
-      <c r="AP8" s="139">
+      <c r="AP8" s="134">
         <f>IFERROR(CORREL($C$4:C8,$S$4:S8),"")</f>
         <v>0.83252878257120233</v>
       </c>
-      <c r="AQ8" s="139">
+      <c r="AQ8" s="134">
         <f>IFERROR(RSQ($C$4:C8,$S$4:S8),"")</f>
         <v>0.69310417380948808</v>
       </c>
-      <c r="AR8" s="139" cm="1">
+      <c r="AR8" s="134" cm="1">
         <f t="array" ref="AR8">IFERROR(_xlfn.STDEV.S($C$4:C8-$S$4:S8)*SQRT(12),"")</f>
         <v>3.0699750390276954E-2</v>
       </c>
-      <c r="AS8" s="139" cm="1">
+      <c r="AS8" s="134" cm="1">
         <f t="array" ref="AS8">IFERROR((AVERAGE($C$4:C8-$S$4:S8)*12)/(_xlfn.STDEV.S($C$4:C8-$S$4:S8)*SQRT(12)),"")</f>
         <v>1.257092550397751</v>
       </c>
-      <c r="AT8" s="139"/>
-      <c r="AU8" s="140"/>
-      <c r="AV8" s="140">
+      <c r="AT8" s="134"/>
+      <c r="AU8" s="135"/>
+      <c r="AV8" s="135">
         <f>S8-AF8</f>
         <v>-4.8293433495903981E-3</v>
       </c>
-      <c r="AW8" s="140">
+      <c r="AW8" s="135">
         <f>U8-(AF8*12)</f>
         <v>-3.5419313196258351E-2</v>
       </c>
-      <c r="AX8" s="139">
+      <c r="AX8" s="134">
         <f t="shared" si="1"/>
         <v>-4.8293433495903981E-3</v>
       </c>
-      <c r="AY8" s="139">
+      <c r="AY8" s="134">
         <f t="shared" si="2"/>
         <v>2.3322557188233006E-5</v>
       </c>
-      <c r="AZ8" s="139" cm="1">
+      <c r="AZ8" s="134" cm="1">
         <f t="array" ref="AZ8">IFERROR(SQRT(AVERAGE(IF($AV$4:AV8&lt;0,($AV$4:AV8)^2,0))),"")</f>
         <v>2.1597480032741322E-3</v>
       </c>
-      <c r="BA8" s="139">
+      <c r="BA8" s="134">
         <f t="shared" si="12"/>
         <v>7.4815865464324619E-3</v>
       </c>
-      <c r="BB8" s="139">
+      <c r="BB8" s="134">
         <f t="shared" si="3"/>
         <v>2.3322557188233006E-5</v>
       </c>
-      <c r="BC8" s="139">
+      <c r="BC8" s="134">
         <f>IFERROR(_xlfn.STDEV.S($AV$4:AV8),"")</f>
         <v>1.5719554490518702E-2</v>
       </c>
-      <c r="BD8" s="139">
+      <c r="BD8" s="134">
         <f t="shared" si="13"/>
         <v>5.4454134099851774E-2</v>
       </c>
-      <c r="BE8" s="140"/>
-      <c r="BF8" s="145"/>
-      <c r="BG8" s="146"/>
-      <c r="BH8" s="147"/>
-      <c r="BI8" s="140">
+      <c r="BE8" s="135"/>
+      <c r="BF8" s="140"/>
+      <c r="BG8" s="141"/>
+      <c r="BH8" s="142"/>
+      <c r="BI8" s="135">
         <f>BN8/BK8</f>
         <v>0.77467030468394726</v>
       </c>
-      <c r="BJ8" s="140">
+      <c r="BJ8" s="135">
         <f>AVERAGE($BI$4:BI8)</f>
         <v>0.71903041066918116</v>
       </c>
-      <c r="BK8" s="148">
+      <c r="BK8" s="143">
         <v>21990000</v>
       </c>
-      <c r="BL8" s="148">
+      <c r="BL8" s="143">
         <v>6370000</v>
       </c>
-      <c r="BM8" s="148">
+      <c r="BM8" s="143">
         <v>4171000</v>
       </c>
-      <c r="BN8" s="148">
+      <c r="BN8" s="143">
         <v>17035000</v>
       </c>
-      <c r="BO8" s="149">
+      <c r="BO8" s="144">
         <v>10574000</v>
       </c>
-      <c r="BP8" s="149">
+      <c r="BP8" s="144">
         <v>2231000</v>
       </c>
-      <c r="BQ8" s="142">
+      <c r="BQ8" s="137">
         <f t="shared" si="14"/>
         <v>0.28967712596634831</v>
       </c>
-      <c r="BR8" s="142">
+      <c r="BR8" s="137">
         <f t="shared" si="15"/>
         <v>-0.18967712596634834</v>
       </c>
-      <c r="BS8" s="142">
+      <c r="BS8" s="137">
         <f>BO8/BK8</f>
         <v>0.48085493406093677</v>
       </c>
-      <c r="BT8" s="142">
+      <c r="BT8" s="137">
         <f>BP8/BK8</f>
         <v>0.10145520691223284</v>
       </c>
-      <c r="BU8" s="142">
+      <c r="BU8" s="137">
         <f>AVERAGE($BS$4:BS8)</f>
         <v>0.47913852384508326</v>
       </c>
-      <c r="BV8" s="142">
+      <c r="BV8" s="137">
         <f>AVERAGE($BT$4:BT8)</f>
         <v>0.18135975013251002</v>
       </c>
-      <c r="BW8" s="150"/>
-      <c r="BX8" s="151" t="s">
+      <c r="BW8" s="145"/>
+      <c r="BX8" s="146" t="s">
         <v>247</v>
       </c>
-      <c r="BY8" s="152" t="e">
+      <c r="BY8" s="147" t="e">
         <f t="shared" ref="BY8" si="19">BZ8/$BZ$11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="BZ8" s="153">
+      <c r="BZ8" s="148">
         <v>1006416.30252</v>
       </c>
       <c r="CB8" s="84" t="e">
         <f>"$500m-$1b (" &amp; TEXT(CC8,"0%") &amp; ")"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="CC8" s="154" t="e" cm="1">
+      <c r="CC8" s="149" t="e" cm="1">
         <f t="array" ref="CC8">SUMPRODUCT((CJ$3:CJ$15&gt;=500000000)*(CJ$3:CJ$15&lt;1000000000)*CK$3:CK$15)</f>
         <v>#DIV/0!</v>
       </c>
@@ -10704,17 +10705,17 @@
       <c r="CF8" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="CG8" s="155">
+      <c r="CG8" s="150">
         <v>4.7334742913622177E-2</v>
       </c>
-      <c r="CI8" s="156" cm="1">
+      <c r="CI8" s="151" cm="1">
         <f t="array" ref="CI8">_xll.BDP(CF8,"CUR_MKT_CAP","CURRENCY","AUD")</f>
         <v>41020148249.550003</v>
       </c>
-      <c r="CJ8" s="156">
+      <c r="CJ8" s="151">
         <v>34799002284.599998</v>
       </c>
-      <c r="CK8" s="157" t="e">
+      <c r="CK8" s="152" t="e">
         <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
@@ -10806,7 +10807,7 @@
         <v>245</v>
       </c>
       <c r="CB9" s="86" t="str">
-        <f t="shared" ref="CB6:CB12" si="20">CA9&amp;"-NYS"</f>
+        <f t="shared" ref="CB9:CB12" si="20">CA9&amp;"-NYS"</f>
         <v>SLB-NYS</v>
       </c>
       <c r="CC9" s="87">
@@ -10825,14 +10826,14 @@
         <v>#NAME?</v>
       </c>
       <c r="CG9" s="88" t="str">
-        <f t="shared" ref="CG3:CG10" ca="1" si="21">IFERROR(CF9*CE9,"")</f>
+        <f t="shared" ref="CG9:CG10" ca="1" si="21">IFERROR(CF9*CE9,"")</f>
         <v/>
       </c>
       <c r="CI9" s="113" t="s">
         <v>107</v>
       </c>
       <c r="CJ9" s="91">
-        <f t="shared" ref="CJ3:CJ10" si="22">CC9/100</f>
+        <f t="shared" ref="CJ9:CJ10" si="22">CC9/100</f>
         <v>3.8280000000000002E-2</v>
       </c>
       <c r="CK9" s="92">
@@ -10848,23 +10849,23 @@
         <v>535.73614122255003</v>
       </c>
       <c r="CO9" s="96">
-        <f t="shared" ref="CO3:CO10" si="23">CN9*CJ9</f>
+        <f t="shared" ref="CO9:CO10" si="23">CN9*CJ9</f>
         <v>20.507979485999215</v>
       </c>
       <c r="CP9" s="97">
-        <f t="shared" ref="CP3:CP12" si="24">CJ9</f>
+        <f t="shared" ref="CP9:CP12" si="24">CJ9</f>
         <v>3.8280000000000002E-2</v>
       </c>
       <c r="CQ9" s="98">
-        <f t="shared" ref="CQ3:CQ12" si="25">CJ9*$CB$35</f>
+        <f t="shared" ref="CQ9:CQ12" si="25">CJ9*$CB$35</f>
         <v>11.484</v>
       </c>
       <c r="CR9" s="98">
-        <f t="shared" ref="CR3:CR12" si="26">CQ9/CN9</f>
+        <f t="shared" ref="CR9:CR12" si="26">CQ9/CN9</f>
         <v>2.1435925479646581E-2</v>
       </c>
       <c r="CS9" s="99">
-        <f t="shared" ref="CS5:CS12" si="27">CS8+1</f>
+        <f t="shared" ref="CS9:CS12" si="27">CS8+1</f>
         <v>1</v>
       </c>
       <c r="CT9" s="112">
@@ -15879,14 +15880,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="BX2:BZ2"/>
+    <mergeCell ref="CB2:CC2"/>
     <mergeCell ref="CA1:CS1"/>
     <mergeCell ref="C1:Q1"/>
     <mergeCell ref="S1:AB1"/>
     <mergeCell ref="AD1:AN1"/>
     <mergeCell ref="AP1:AX1"/>
     <mergeCell ref="AZ1:BN1"/>
-    <mergeCell ref="BX2:BZ2"/>
-    <mergeCell ref="CB2:CC2"/>
   </mergeCells>
   <conditionalFormatting sqref="DC3:DF39 DH3:DT39">
     <cfRule type="expression" dxfId="0" priority="2">
@@ -16150,7 +16151,7 @@
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="171">
+      <c r="B2" s="164">
         <v>3.3316831683168235E-2</v>
       </c>
     </row>
@@ -16158,7 +16159,7 @@
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="171">
+      <c r="B3" s="164">
         <v>-2.7000943758537232E-3</v>
       </c>
     </row>
@@ -16166,7 +16167,7 @@
       <c r="A4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="171">
+      <c r="B4" s="164">
         <v>3.5027275337352837E-2</v>
       </c>
     </row>
@@ -16174,7 +16175,7 @@
       <c r="A5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="171">
+      <c r="B5" s="164">
         <v>-1.8777339165688689E-3</v>
       </c>
     </row>
@@ -16352,14 +16353,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" customWidth="1"/>
     <col min="5" max="5" width="17.81640625" customWidth="1"/>
     <col min="7" max="7" width="17.453125" customWidth="1"/>
     <col min="8" max="8" width="34.453125" customWidth="1"/>
@@ -16396,7 +16397,7 @@
       <c r="B2" s="120">
         <v>0.52400000000000002</v>
       </c>
-      <c r="D2" s="109" t="s">
+      <c r="D2" s="165" t="s">
         <v>91</v>
       </c>
       <c r="E2">
@@ -16419,7 +16420,7 @@
       <c r="B3" s="120">
         <v>-1.9900000000000001E-2</v>
       </c>
-      <c r="D3" s="109" t="s">
+      <c r="D3" s="165" t="s">
         <v>279</v>
       </c>
       <c r="E3">
@@ -16444,7 +16445,7 @@
         <f>B2+B3</f>
         <v>0.50409999999999999</v>
       </c>
-      <c r="D4" s="109" t="s">
+      <c r="D4" s="165" t="s">
         <v>92</v>
       </c>
       <c r="E4">
@@ -16461,7 +16462,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="D5" t="s">
+      <c r="D5" s="165" t="s">
         <v>286</v>
       </c>
       <c r="E5">
@@ -16479,7 +16480,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="D6" s="109" t="s">
+      <c r="D6" s="165" t="s">
         <v>114</v>
       </c>
       <c r="E6">
@@ -16562,7 +16563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
@@ -16665,15 +16666,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100693564D6C4D0CB46BB0B3867B66CB08A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c319d8763b72b8751faf181ae4ae768f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cd6d0250-26e6-4018-96cc-9d4b267bf602" xmlns:ns3="ba7ac31c-47df-4cec-a670-87c4a6b08e03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="84d0083d4454dea4e9840a7b60f9a3ce" ns2:_="" ns3:_="">
     <xsd:import namespace="cd6d0250-26e6-4018-96cc-9d4b267bf602"/>
@@ -16874,7 +16866,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="cd6d0250-26e6-4018-96cc-9d4b267bf602">
@@ -16886,15 +16878,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA5DAC66-34FF-411F-B27D-494581287E7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7566D01C-ECEC-4BF5-8616-12E76A91A7FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16913,7 +16906,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CDF4DAF-E893-439E-B96A-FDDC553C23F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -16922,4 +16915,12 @@
     <ds:schemaRef ds:uri="ba7ac31c-47df-4cec-a670-87c4a6b08e03"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA5DAC66-34FF-411F-B27D-494581287E7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add date updated information to performance data
Update performance.js to read and return the `dateUpdated` field from the Excel file, modifying the `/performance` endpoint response to include this new data point.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 54b95f43-839d-43a1-b23c-b8a21fe56cf6
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: f059ff95-ece0-46f3-963b-af8b60de4f0c
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f473309e-b340-4b77-bcdf-327a8eec9336/54b95f43-839d-43a1-b23c-b8a21fe56cf6/ci5aVcl
</commit_message>
<xml_diff>
--- a/LaserBeamExcel.xlsx
+++ b/LaserBeamExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://laserbeamptyltd.sharepoint.com/sites/LaserBeamCapital2/Shared Documents/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{5F60E2F0-575E-4A08-ABF9-32171979650C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53CE5253-0087-4283-9C94-44E87C04350C}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{5F60E2F0-575E-4A08-ABF9-32171979650C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5771922-FA08-4358-BB43-B155F46088AE}"/>
   <bookViews>
-    <workbookView xWindow="21168" yWindow="1380" windowWidth="24864" windowHeight="23628" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21228" yWindow="972" windowWidth="24864" windowHeight="23628" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions - New month" sheetId="1" state="hidden" r:id="rId1"/>
@@ -29,6 +29,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xleta.GROWTH" hidden="1">#NAME?</definedName>
+    <definedName name="Date_updated">Performance!$G$1:$G$2</definedName>
     <definedName name="MarketCapExposureTable">Exposure!$G$1:$I$6</definedName>
     <definedName name="NetExposureTable">Exposure!$A$1:$B$4</definedName>
     <definedName name="PerformanceChartTable">Table1[#All]</definedName>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="290">
   <si>
     <t>1. update the separate fund spreadsheets in "Newsletter Data &gt; Convserions" for the latest months performance</t>
   </si>
@@ -960,12 +961,15 @@
   <si>
     <t>Unity Software</t>
   </si>
+  <si>
+    <t>Date updated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="20">
+  <numFmts count="21">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
@@ -986,6 +990,7 @@
     <numFmt numFmtId="180" formatCode="&quot;$&quot;###&quot;m&quot;"/>
     <numFmt numFmtId="181" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="182" formatCode="[$-10409]#,##0.00;\(#,##0.00\);&quot;-&quot;"/>
+    <numFmt numFmtId="185" formatCode="d\ mmm"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1391,7 +1396,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="21" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1813,11 +1818,11 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="37" fillId="13" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1831,6 +1836,7 @@
     <xf numFmtId="166" fontId="21" fillId="5" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1961,8 +1967,8 @@
         <v>#N/A Requesting Data...3051439136</v>
         <stp/>
         <stp>BDP|4639078413468701993</stp>
+        <tr r="CI8" s="3"/>
         <tr r="CI7" s="3"/>
-        <tr r="CI8" s="3"/>
       </tp>
       <tp t="s">
         <v>#N/A Requesting Data...3590692652</v>
@@ -7311,6 +7317,9 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table7" displayName="Table7" ref="D1:E10" totalsRowShown="0">
   <autoFilter ref="D1:E10" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E10">
+    <sortCondition descending="1" ref="E2:E10"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="value"/>
@@ -7651,11 +7660,11 @@
     </row>
     <row r="18" spans="2:15" ht="40.5" customHeight="1">
       <c r="B18" s="11"/>
-      <c r="D18" s="168" t="s">
+      <c r="D18" s="167" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="168"/>
-      <c r="F18" s="168"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="167"/>
       <c r="G18" s="12"/>
       <c r="H18" s="3">
         <f>INDEX(Performancedata!C:C, MATCH(A2, Performancedata!A:A, 0))</f>
@@ -8072,41 +8081,41 @@
       <c r="AF111" s="10"/>
     </row>
     <row r="112" spans="19:32" ht="27.75" customHeight="1">
-      <c r="S112" s="167" t="s">
+      <c r="S112" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="T112" s="167"/>
+      <c r="T112" s="168"/>
       <c r="U112" s="30"/>
       <c r="V112" s="31"/>
       <c r="W112" s="31"/>
-      <c r="X112" s="167" t="s">
+      <c r="X112" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="Y112" s="167"/>
+      <c r="Y112" s="168"/>
       <c r="Z112" s="31"/>
       <c r="AA112" s="31"/>
       <c r="AB112" s="31"/>
-      <c r="AC112" s="167" t="s">
+      <c r="AC112" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="AD112" s="167"/>
+      <c r="AD112" s="168"/>
       <c r="AE112" s="31"/>
       <c r="AF112" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="113" spans="19:33" ht="18.75" customHeight="1">
-      <c r="S113" s="167" t="s">
+      <c r="S113" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="T113" s="167"/>
+      <c r="T113" s="168"/>
       <c r="U113" s="30"/>
       <c r="V113" s="31"/>
       <c r="W113" s="31"/>
-      <c r="X113" s="167" t="s">
+      <c r="X113" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="Y113" s="167"/>
+      <c r="Y113" s="168"/>
       <c r="Z113" s="31"/>
       <c r="AA113" s="31"/>
       <c r="AB113" s="31"/>
@@ -8120,17 +8129,17 @@
       </c>
     </row>
     <row r="114" spans="19:33" ht="18.75" customHeight="1">
-      <c r="S114" s="167" t="s">
+      <c r="S114" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="T114" s="167"/>
+      <c r="T114" s="168"/>
       <c r="U114" s="30"/>
       <c r="V114" s="31"/>
       <c r="W114" s="31"/>
-      <c r="X114" s="167" t="s">
+      <c r="X114" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="Y114" s="167"/>
+      <c r="Y114" s="168"/>
       <c r="Z114" s="31"/>
       <c r="AA114" s="31"/>
       <c r="AB114" s="31"/>
@@ -8144,17 +8153,17 @@
       </c>
     </row>
     <row r="115" spans="19:33" ht="21.75" customHeight="1">
-      <c r="S115" s="167" t="s">
+      <c r="S115" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="T115" s="167"/>
+      <c r="T115" s="168"/>
       <c r="U115" s="45"/>
       <c r="V115" s="46"/>
       <c r="W115" s="46"/>
-      <c r="X115" s="167" t="s">
+      <c r="X115" s="168" t="s">
         <v>18</v>
       </c>
-      <c r="Y115" s="167"/>
+      <c r="Y115" s="168"/>
       <c r="Z115" s="46"/>
       <c r="AA115" s="47"/>
       <c r="AB115" s="46"/>
@@ -8595,16 +8604,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="K59:N59"/>
-    <mergeCell ref="S112:T112"/>
-    <mergeCell ref="X112:Y112"/>
-    <mergeCell ref="AC112:AD112"/>
-    <mergeCell ref="S113:T113"/>
-    <mergeCell ref="X113:Y113"/>
     <mergeCell ref="AC125:AF125"/>
     <mergeCell ref="S131:V131"/>
     <mergeCell ref="S114:T114"/>
@@ -8613,6 +8612,16 @@
     <mergeCell ref="X115:Y115"/>
     <mergeCell ref="S125:V125"/>
     <mergeCell ref="X125:AA125"/>
+    <mergeCell ref="S112:T112"/>
+    <mergeCell ref="X112:Y112"/>
+    <mergeCell ref="AC112:AD112"/>
+    <mergeCell ref="S113:T113"/>
+    <mergeCell ref="X113:Y113"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="K59:N59"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="3.9583333333333297E-2" right="3.9583333333333297E-2" top="3.9583333333333297E-2" bottom="7.8472222222222193E-2" header="0.511811023622047" footer="0.511811023622047"/>
@@ -8626,7 +8635,7 @@
   <dimension ref="A1:ED61"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BR37" sqref="BR37"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.25" customHeight="1"/>
@@ -15902,10 +15911,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.25" customHeight="1"/>
@@ -15913,9 +15922,10 @@
     <col min="1" max="1" width="12.81640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="5" max="5" width="34.26953125" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.5">
+    <row r="1" spans="1:7" ht="14.5">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -15928,8 +15938,11 @@
       <c r="E1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="14.5">
+      <c r="G1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.5">
       <c r="A2" s="118">
         <v>45838</v>
       </c>
@@ -15943,8 +15956,11 @@
         <f>Performancedata!C8</f>
         <v>-2.7000943758537232E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="14.5">
+      <c r="G2" s="173">
+        <v>45991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.5">
       <c r="A3" s="118">
         <v>45869</v>
       </c>
@@ -15959,7 +15975,7 @@
         <v>6.340400929875023E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.5">
+    <row r="4" spans="1:7" ht="14.5">
       <c r="A4" s="118">
         <v>45900</v>
       </c>
@@ -15974,7 +15990,7 @@
         <v>0.11699957136740702</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.5">
+    <row r="5" spans="1:7" ht="14.5">
       <c r="A5" s="118">
         <v>45930</v>
       </c>
@@ -15989,7 +16005,7 @@
         <v>0.30433888942018061</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1">
       <c r="A6" s="131">
         <v>45961</v>
       </c>
@@ -15998,7 +16014,7 @@
         <v>0.12002374117176751</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="131">
         <v>45991</v>
       </c>
@@ -16353,8 +16369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.25" customHeight="1"/>
@@ -16398,10 +16414,10 @@
         <v>0.52400000000000002</v>
       </c>
       <c r="D2" s="165" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="E2">
-        <v>0.13789999999999999</v>
+        <v>0.62</v>
       </c>
       <c r="G2" t="s">
         <v>229</v>
@@ -16421,11 +16437,10 @@
         <v>-1.9900000000000001E-2</v>
       </c>
       <c r="D3" s="165" t="s">
-        <v>279</v>
+        <v>91</v>
       </c>
       <c r="E3">
-        <f>0.1379-0.0598</f>
-        <v>7.8100000000000003E-2</v>
+        <v>0.13789999999999999</v>
       </c>
       <c r="G3" t="s">
         <v>231</v>
@@ -16463,11 +16478,11 @@
     </row>
     <row r="5" spans="1:9">
       <c r="D5" s="165" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E5">
-        <f>1-E6-E4-E3-E2</f>
-        <v>5.400000000000002E-2</v>
+        <f>0.1379-0.0598</f>
+        <v>7.8100000000000003E-2</v>
       </c>
       <c r="G5" t="s">
         <v>234</v>
@@ -16481,10 +16496,11 @@
     </row>
     <row r="6" spans="1:9">
       <c r="D6" s="165" t="s">
-        <v>114</v>
+        <v>286</v>
       </c>
       <c r="E6">
-        <v>0.62</v>
+        <f>1-SUM(E2:E5)</f>
+        <v>5.4000000000000048E-2</v>
       </c>
       <c r="G6" t="s">
         <v>235</v>
@@ -16867,6 +16883,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="cd6d0250-26e6-4018-96cc-9d4b267bf602">
@@ -16876,15 +16901,6 @@
     <MediaLengthInSeconds xmlns="cd6d0250-26e6-4018-96cc-9d4b267bf602" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16907,6 +16923,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA5DAC66-34FF-411F-B27D-494581287E7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CDF4DAF-E893-439E-B96A-FDDC553C23F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -16915,12 +16939,4 @@
     <ds:schemaRef ds:uri="ba7ac31c-47df-4cec-a670-87c4a6b08e03"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA5DAC66-34FF-411F-B27D-494581287E7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>